<commit_message>
Day 8 DS Topics
</commit_message>
<xml_diff>
--- a/CP_Platform_Solution_.Net_v1.4-Phase1.xlsx
+++ b/CP_Platform_Solution_.Net_v1.4-Phase1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anami\Wipro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE61CFE3-9892-4120-9477-DCC81252BEDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D853E5-BBA3-496A-9C75-793EC3F22448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" activeTab="2" xr2:uid="{A334C00E-DF14-8E42-AC33-43AB2B07B0C8}"/>
   </bookViews>
@@ -2177,24 +2177,60 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
@@ -2204,14 +2240,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="7"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2225,86 +2261,50 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2722,16 +2722,16 @@
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A2" s="18" t="s">
@@ -2750,13 +2750,13 @@
       <c r="A4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
       <c r="G4" s="19" t="s">
         <v>6</v>
       </c>
@@ -2771,187 +2771,187 @@
       <c r="A5" s="20">
         <v>1</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="41" t="s">
         <v>172</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="64" t="s">
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="44" t="s">
         <v>173</v>
       </c>
-      <c r="H5" s="64" t="s">
+      <c r="H5" s="44" t="s">
         <v>174</v>
       </c>
-      <c r="I5" s="55">
+      <c r="I5" s="47">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A6" s="39">
+      <c r="A6" s="50">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="56" t="s">
         <v>175</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="56"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="48"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A7" s="40"/>
-      <c r="B7" s="45" t="s">
+      <c r="A7" s="51"/>
+      <c r="B7" s="57" t="s">
         <v>176</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="56"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="48"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A8" s="40"/>
-      <c r="B8" s="45" t="s">
+      <c r="A8" s="51"/>
+      <c r="B8" s="57" t="s">
         <v>177</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="56"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="48"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A9" s="40"/>
-      <c r="B9" s="45" t="s">
+      <c r="A9" s="51"/>
+      <c r="B9" s="57" t="s">
         <v>178</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="65"/>
-      <c r="H9" s="65"/>
-      <c r="I9" s="56"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="48"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A10" s="40"/>
-      <c r="B10" s="45" t="s">
+      <c r="A10" s="51"/>
+      <c r="B10" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="65"/>
-      <c r="H10" s="65"/>
-      <c r="I10" s="56"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="48"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A11" s="40"/>
-      <c r="B11" s="59" t="s">
+      <c r="A11" s="51"/>
+      <c r="B11" s="60" t="s">
         <v>180</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="56"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="48"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A12" s="41"/>
-      <c r="B12" s="59" t="s">
+      <c r="A12" s="55"/>
+      <c r="B12" s="60" t="s">
         <v>181</v>
       </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="65"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="56"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="48"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A13" s="39">
+      <c r="A13" s="50">
         <v>1.2</v>
       </c>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="52" t="s">
         <v>182</v>
       </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="56"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="48"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A14" s="40"/>
-      <c r="B14" s="45" t="s">
+      <c r="A14" s="51"/>
+      <c r="B14" s="57" t="s">
         <v>183</v>
       </c>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="56"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="48"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A15" s="40"/>
-      <c r="B15" s="45" t="s">
+      <c r="A15" s="51"/>
+      <c r="B15" s="57" t="s">
         <v>184</v>
       </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="56"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="48"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A16" s="41"/>
-      <c r="B16" s="45" t="s">
+      <c r="A16" s="55"/>
+      <c r="B16" s="57" t="s">
         <v>185</v>
       </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="56"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="48"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A17" s="39">
+      <c r="A17" s="50">
         <v>1.3</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="56"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="48"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A18" s="40"/>
+      <c r="A18" s="51"/>
       <c r="B18" s="25" t="s">
         <v>187</v>
       </c>
@@ -2959,12 +2959,12 @@
       <c r="D18" s="26"/>
       <c r="E18" s="26"/>
       <c r="F18" s="27"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="56"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="48"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A19" s="40"/>
+      <c r="A19" s="51"/>
       <c r="B19" s="25" t="s">
         <v>188</v>
       </c>
@@ -2972,318 +2972,318 @@
       <c r="D19" s="26"/>
       <c r="E19" s="26"/>
       <c r="F19" s="27"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="65"/>
-      <c r="I19" s="56"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="48"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A20" s="39">
+      <c r="A20" s="50">
         <v>1.4</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="56" t="s">
         <v>189</v>
       </c>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="65"/>
-      <c r="H20" s="65"/>
-      <c r="I20" s="56"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="48"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A21" s="40"/>
-      <c r="B21" s="45" t="s">
+      <c r="A21" s="51"/>
+      <c r="B21" s="57" t="s">
         <v>190</v>
       </c>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="65"/>
-      <c r="I21" s="56"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="48"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A22" s="40"/>
-      <c r="B22" s="45" t="s">
+      <c r="A22" s="51"/>
+      <c r="B22" s="57" t="s">
         <v>191</v>
       </c>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="65"/>
-      <c r="H22" s="65"/>
-      <c r="I22" s="56"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="48"/>
     </row>
     <row r="23" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A23" s="41"/>
-      <c r="B23" s="45" t="s">
+      <c r="A23" s="55"/>
+      <c r="B23" s="57" t="s">
         <v>192</v>
       </c>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="65"/>
-      <c r="I23" s="56"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="48"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A24" s="39">
+      <c r="A24" s="50">
         <v>1.5</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="56" t="s">
         <v>193</v>
       </c>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="56"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="48"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A25" s="40"/>
-      <c r="B25" s="45" t="s">
+      <c r="A25" s="51"/>
+      <c r="B25" s="57" t="s">
         <v>194</v>
       </c>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="65"/>
-      <c r="I25" s="56"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="48"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A26" s="40"/>
-      <c r="B26" s="45" t="s">
+      <c r="A26" s="51"/>
+      <c r="B26" s="57" t="s">
         <v>195</v>
       </c>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="65"/>
-      <c r="H26" s="65"/>
-      <c r="I26" s="56"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="48"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A27" s="41"/>
-      <c r="B27" s="45" t="s">
+      <c r="A27" s="55"/>
+      <c r="B27" s="57" t="s">
         <v>196</v>
       </c>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="66"/>
-      <c r="I27" s="57"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="49"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A28" s="20">
         <v>2</v>
       </c>
-      <c r="B28" s="48" t="s">
+      <c r="B28" s="41" t="s">
         <v>197</v>
       </c>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="51" t="s">
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="63" t="s">
         <v>198</v>
       </c>
-      <c r="H28" s="54" t="s">
+      <c r="H28" s="66" t="s">
         <v>199</v>
       </c>
-      <c r="I28" s="55">
+      <c r="I28" s="47">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A29" s="39">
+      <c r="A29" s="50">
         <v>2.1</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="56" t="s">
         <v>200</v>
       </c>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="52"/>
-      <c r="I29" s="56"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="54"/>
+      <c r="G29" s="64"/>
+      <c r="H29" s="64"/>
+      <c r="I29" s="48"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A30" s="40"/>
-      <c r="B30" s="45" t="s">
+      <c r="A30" s="51"/>
+      <c r="B30" s="57" t="s">
         <v>201</v>
       </c>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="56"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="64"/>
+      <c r="H30" s="64"/>
+      <c r="I30" s="48"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A31" s="40"/>
-      <c r="B31" s="45" t="s">
+      <c r="A31" s="51"/>
+      <c r="B31" s="57" t="s">
         <v>202</v>
       </c>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="56"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="64"/>
+      <c r="H31" s="64"/>
+      <c r="I31" s="48"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A32" s="41"/>
-      <c r="B32" s="45" t="s">
+      <c r="A32" s="55"/>
+      <c r="B32" s="57" t="s">
         <v>203</v>
       </c>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="56"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="64"/>
+      <c r="H32" s="64"/>
+      <c r="I32" s="48"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A33" s="39">
+      <c r="A33" s="50">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="56" t="s">
         <v>204</v>
       </c>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="52"/>
-      <c r="H33" s="52"/>
-      <c r="I33" s="56"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="54"/>
+      <c r="G33" s="64"/>
+      <c r="H33" s="64"/>
+      <c r="I33" s="48"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A34" s="40"/>
-      <c r="B34" s="45" t="s">
+      <c r="A34" s="51"/>
+      <c r="B34" s="57" t="s">
         <v>205</v>
       </c>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="56"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="58"/>
+      <c r="F34" s="59"/>
+      <c r="G34" s="64"/>
+      <c r="H34" s="64"/>
+      <c r="I34" s="48"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A35" s="40"/>
-      <c r="B35" s="45" t="s">
+      <c r="A35" s="51"/>
+      <c r="B35" s="57" t="s">
         <v>206</v>
       </c>
-      <c r="C35" s="46"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="46"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="52"/>
-      <c r="H35" s="52"/>
-      <c r="I35" s="56"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="58"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="64"/>
+      <c r="H35" s="64"/>
+      <c r="I35" s="48"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A36" s="41"/>
-      <c r="B36" s="45" t="s">
+      <c r="A36" s="55"/>
+      <c r="B36" s="57" t="s">
         <v>207</v>
       </c>
-      <c r="C36" s="46"/>
-      <c r="D36" s="46"/>
-      <c r="E36" s="46"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="52"/>
-      <c r="H36" s="52"/>
-      <c r="I36" s="56"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="64"/>
+      <c r="H36" s="64"/>
+      <c r="I36" s="48"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A37" s="39">
+      <c r="A37" s="50">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B37" s="42" t="s">
+      <c r="B37" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="C37" s="43"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="52"/>
-      <c r="I37" s="56"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="54"/>
+      <c r="G37" s="64"/>
+      <c r="H37" s="64"/>
+      <c r="I37" s="48"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A38" s="40"/>
-      <c r="B38" s="45" t="s">
+      <c r="A38" s="51"/>
+      <c r="B38" s="57" t="s">
         <v>209</v>
       </c>
-      <c r="C38" s="46"/>
-      <c r="D38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="52"/>
-      <c r="H38" s="52"/>
-      <c r="I38" s="56"/>
+      <c r="C38" s="58"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="58"/>
+      <c r="F38" s="59"/>
+      <c r="G38" s="64"/>
+      <c r="H38" s="64"/>
+      <c r="I38" s="48"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A39" s="40"/>
-      <c r="B39" s="45" t="s">
+      <c r="A39" s="51"/>
+      <c r="B39" s="57" t="s">
         <v>210</v>
       </c>
-      <c r="C39" s="46"/>
-      <c r="D39" s="46"/>
-      <c r="E39" s="46"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="52"/>
-      <c r="H39" s="52"/>
-      <c r="I39" s="56"/>
+      <c r="C39" s="58"/>
+      <c r="D39" s="58"/>
+      <c r="E39" s="58"/>
+      <c r="F39" s="59"/>
+      <c r="G39" s="64"/>
+      <c r="H39" s="64"/>
+      <c r="I39" s="48"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A40" s="41"/>
-      <c r="B40" s="45" t="s">
+      <c r="A40" s="55"/>
+      <c r="B40" s="57" t="s">
         <v>211</v>
       </c>
-      <c r="C40" s="46"/>
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="52"/>
-      <c r="H40" s="52"/>
-      <c r="I40" s="56"/>
+      <c r="C40" s="58"/>
+      <c r="D40" s="58"/>
+      <c r="E40" s="58"/>
+      <c r="F40" s="59"/>
+      <c r="G40" s="64"/>
+      <c r="H40" s="64"/>
+      <c r="I40" s="48"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A41" s="39">
+      <c r="A41" s="50">
         <v>2.4</v>
       </c>
-      <c r="B41" s="42" t="s">
+      <c r="B41" s="56" t="s">
         <v>212</v>
       </c>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="44"/>
-      <c r="G41" s="52"/>
-      <c r="H41" s="52"/>
-      <c r="I41" s="56"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="53"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="64"/>
+      <c r="H41" s="64"/>
+      <c r="I41" s="48"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A42" s="40"/>
+      <c r="A42" s="51"/>
       <c r="B42" s="25" t="s">
         <v>213</v>
       </c>
@@ -3291,12 +3291,12 @@
       <c r="D42" s="26"/>
       <c r="E42" s="26"/>
       <c r="F42" s="27"/>
-      <c r="G42" s="52"/>
-      <c r="H42" s="52"/>
-      <c r="I42" s="56"/>
+      <c r="G42" s="64"/>
+      <c r="H42" s="64"/>
+      <c r="I42" s="48"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A43" s="41"/>
+      <c r="A43" s="55"/>
       <c r="B43" s="25" t="s">
         <v>214</v>
       </c>
@@ -3304,27 +3304,27 @@
       <c r="D43" s="26"/>
       <c r="E43" s="26"/>
       <c r="F43" s="27"/>
-      <c r="G43" s="52"/>
-      <c r="H43" s="52"/>
-      <c r="I43" s="56"/>
+      <c r="G43" s="64"/>
+      <c r="H43" s="64"/>
+      <c r="I43" s="48"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A44" s="39">
+      <c r="A44" s="50">
         <v>2.5</v>
       </c>
-      <c r="B44" s="42" t="s">
+      <c r="B44" s="56" t="s">
         <v>215</v>
       </c>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="52"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="56"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="54"/>
+      <c r="G44" s="64"/>
+      <c r="H44" s="64"/>
+      <c r="I44" s="48"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A45" s="40"/>
+      <c r="A45" s="51"/>
       <c r="B45" s="25" t="s">
         <v>216</v>
       </c>
@@ -3332,12 +3332,12 @@
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="27"/>
-      <c r="G45" s="52"/>
-      <c r="H45" s="52"/>
-      <c r="I45" s="56"/>
+      <c r="G45" s="64"/>
+      <c r="H45" s="64"/>
+      <c r="I45" s="48"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A46" s="41"/>
+      <c r="A46" s="55"/>
       <c r="B46" s="25" t="s">
         <v>217</v>
       </c>
@@ -3345,97 +3345,78 @@
       <c r="D46" s="26"/>
       <c r="E46" s="26"/>
       <c r="F46" s="27"/>
-      <c r="G46" s="52"/>
-      <c r="H46" s="52"/>
-      <c r="I46" s="56"/>
+      <c r="G46" s="64"/>
+      <c r="H46" s="64"/>
+      <c r="I46" s="48"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A47" s="39">
+      <c r="A47" s="50">
         <v>2.6</v>
       </c>
-      <c r="B47" s="42" t="s">
+      <c r="B47" s="56" t="s">
         <v>218</v>
       </c>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="44"/>
-      <c r="G47" s="52"/>
-      <c r="H47" s="52"/>
-      <c r="I47" s="56"/>
+      <c r="C47" s="53"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="53"/>
+      <c r="F47" s="54"/>
+      <c r="G47" s="64"/>
+      <c r="H47" s="64"/>
+      <c r="I47" s="48"/>
     </row>
     <row r="48" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A48" s="40"/>
-      <c r="B48" s="45" t="s">
+      <c r="A48" s="51"/>
+      <c r="B48" s="57" t="s">
         <v>219</v>
       </c>
-      <c r="C48" s="46"/>
-      <c r="D48" s="46"/>
-      <c r="E48" s="46"/>
-      <c r="F48" s="47"/>
-      <c r="G48" s="52"/>
-      <c r="H48" s="52"/>
-      <c r="I48" s="56"/>
+      <c r="C48" s="58"/>
+      <c r="D48" s="58"/>
+      <c r="E48" s="58"/>
+      <c r="F48" s="59"/>
+      <c r="G48" s="64"/>
+      <c r="H48" s="64"/>
+      <c r="I48" s="48"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A49" s="40"/>
-      <c r="B49" s="45" t="s">
+      <c r="A49" s="51"/>
+      <c r="B49" s="57" t="s">
         <v>220</v>
       </c>
-      <c r="C49" s="46"/>
-      <c r="D49" s="46"/>
-      <c r="E49" s="46"/>
-      <c r="F49" s="47"/>
-      <c r="G49" s="52"/>
-      <c r="H49" s="52"/>
-      <c r="I49" s="56"/>
+      <c r="C49" s="58"/>
+      <c r="D49" s="58"/>
+      <c r="E49" s="58"/>
+      <c r="F49" s="59"/>
+      <c r="G49" s="64"/>
+      <c r="H49" s="64"/>
+      <c r="I49" s="48"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A50" s="41"/>
-      <c r="B50" s="45" t="s">
+      <c r="A50" s="55"/>
+      <c r="B50" s="57" t="s">
         <v>221</v>
       </c>
-      <c r="C50" s="46"/>
-      <c r="D50" s="46"/>
-      <c r="E50" s="46"/>
-      <c r="F50" s="47"/>
-      <c r="G50" s="53"/>
-      <c r="H50" s="53"/>
-      <c r="I50" s="57"/>
+      <c r="C50" s="58"/>
+      <c r="D50" s="58"/>
+      <c r="E50" s="58"/>
+      <c r="F50" s="59"/>
+      <c r="G50" s="65"/>
+      <c r="H50" s="65"/>
+      <c r="I50" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="G5:G27"/>
-    <mergeCell ref="H5:H27"/>
-    <mergeCell ref="I5:I27"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:F41"/>
     <mergeCell ref="B28:F28"/>
     <mergeCell ref="G28:G50"/>
     <mergeCell ref="H28:H50"/>
@@ -3452,18 +3433,37 @@
     <mergeCell ref="B36:F36"/>
     <mergeCell ref="A37:A40"/>
     <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="G5:G27"/>
+    <mergeCell ref="H5:H27"/>
+    <mergeCell ref="I5:I27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3479,8 +3479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E4222C-B6F0-CA43-929A-A25489896A98}">
   <dimension ref="A1:G161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50:C98"/>
+    <sheetView tabSelected="1" topLeftCell="D80" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G99" sqref="G99:G141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -3496,11 +3496,11 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="81" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A2" s="8" t="s">
@@ -3539,179 +3539,179 @@
       <c r="B5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="71" t="s">
         <v>155</v>
       </c>
-      <c r="D5" s="70">
+      <c r="D5" s="80">
         <v>1</v>
       </c>
       <c r="E5" s="17"/>
-      <c r="G5" s="74" t="s">
+      <c r="G5" s="76" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="71">
+      <c r="A6" s="79">
         <v>1.1000000000000001</v>
       </c>
       <c r="B6" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="69"/>
-      <c r="D6" s="70"/>
-      <c r="G6" s="75"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="80"/>
+      <c r="G6" s="77"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A7" s="71"/>
+      <c r="A7" s="79"/>
       <c r="B7" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="69"/>
-      <c r="D7" s="70"/>
-      <c r="G7" s="75"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="80"/>
+      <c r="G7" s="77"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A8" s="71"/>
+      <c r="A8" s="79"/>
       <c r="B8" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="69"/>
-      <c r="D8" s="70"/>
-      <c r="G8" s="75"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="80"/>
+      <c r="G8" s="77"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A9" s="71"/>
+      <c r="A9" s="79"/>
       <c r="B9" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="69"/>
-      <c r="D9" s="70"/>
-      <c r="G9" s="75"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="80"/>
+      <c r="G9" s="77"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A10" s="71">
+      <c r="A10" s="79">
         <v>1.2</v>
       </c>
       <c r="B10" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="69"/>
-      <c r="D10" s="70"/>
-      <c r="G10" s="75"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="80"/>
+      <c r="G10" s="77"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A11" s="71"/>
+      <c r="A11" s="79"/>
       <c r="B11" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="70"/>
-      <c r="G11" s="75"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="80"/>
+      <c r="G11" s="77"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A12" s="71"/>
+      <c r="A12" s="79"/>
       <c r="B12" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="69"/>
-      <c r="D12" s="70"/>
-      <c r="G12" s="75"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="80"/>
+      <c r="G12" s="77"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A13" s="71">
+      <c r="A13" s="79">
         <v>1.3</v>
       </c>
       <c r="B13" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="69"/>
-      <c r="D13" s="70"/>
-      <c r="G13" s="75"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="80"/>
+      <c r="G13" s="77"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A14" s="71"/>
+      <c r="A14" s="79"/>
       <c r="B14" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="69"/>
-      <c r="D14" s="70"/>
-      <c r="G14" s="75"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="80"/>
+      <c r="G14" s="77"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A15" s="71"/>
+      <c r="A15" s="79"/>
       <c r="B15" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="69"/>
-      <c r="D15" s="70"/>
-      <c r="G15" s="75"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="80"/>
+      <c r="G15" s="77"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A16" s="71"/>
+      <c r="A16" s="79"/>
       <c r="B16" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="69"/>
-      <c r="D16" s="70"/>
-      <c r="G16" s="75"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="80"/>
+      <c r="G16" s="77"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A17" s="71">
+      <c r="A17" s="79">
         <v>1.4</v>
       </c>
       <c r="B17" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="69"/>
-      <c r="D17" s="70"/>
-      <c r="G17" s="75"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="80"/>
+      <c r="G17" s="77"/>
     </row>
     <row r="18" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A18" s="71"/>
+      <c r="A18" s="79"/>
       <c r="B18" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="69"/>
-      <c r="D18" s="70"/>
-      <c r="G18" s="75"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="80"/>
+      <c r="G18" s="77"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A19" s="71"/>
+      <c r="A19" s="79"/>
       <c r="B19" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="69"/>
-      <c r="D19" s="70"/>
-      <c r="G19" s="75"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="80"/>
+      <c r="G19" s="77"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A20" s="71">
+      <c r="A20" s="79">
         <v>1.5</v>
       </c>
       <c r="B20" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="69"/>
-      <c r="D20" s="70"/>
-      <c r="G20" s="75"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="80"/>
+      <c r="G20" s="77"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A21" s="71"/>
+      <c r="A21" s="79"/>
       <c r="B21" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="69"/>
-      <c r="D21" s="70"/>
-      <c r="G21" s="75"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="80"/>
+      <c r="G21" s="77"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A22" s="71"/>
+      <c r="A22" s="79"/>
       <c r="B22" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="69"/>
-      <c r="D22" s="70"/>
-      <c r="G22" s="75"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="80"/>
+      <c r="G22" s="77"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A23" s="6">
@@ -3720,38 +3720,38 @@
       <c r="B23" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="69"/>
-      <c r="D23" s="70"/>
-      <c r="G23" s="75"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="80"/>
+      <c r="G23" s="77"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A24" s="71">
+      <c r="A24" s="79">
         <v>2.1</v>
       </c>
       <c r="B24" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="69"/>
-      <c r="D24" s="70"/>
-      <c r="G24" s="75"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="80"/>
+      <c r="G24" s="77"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A25" s="71"/>
+      <c r="A25" s="79"/>
       <c r="B25" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="69"/>
-      <c r="D25" s="70"/>
-      <c r="G25" s="75"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="80"/>
+      <c r="G25" s="77"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A26" s="71"/>
+      <c r="A26" s="79"/>
       <c r="B26" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="69"/>
-      <c r="D26" s="70"/>
-      <c r="G26" s="75"/>
+      <c r="C26" s="71"/>
+      <c r="D26" s="80"/>
+      <c r="G26" s="77"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A27" s="67">
@@ -3760,36 +3760,36 @@
       <c r="B27" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="69"/>
-      <c r="D27" s="70"/>
-      <c r="G27" s="75"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="80"/>
+      <c r="G27" s="77"/>
     </row>
     <row r="28" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A28" s="67"/>
       <c r="B28" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="69"/>
-      <c r="D28" s="70"/>
-      <c r="G28" s="75"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="80"/>
+      <c r="G28" s="77"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A29" s="67"/>
       <c r="B29" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="69"/>
-      <c r="D29" s="70"/>
-      <c r="G29" s="75"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="80"/>
+      <c r="G29" s="77"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A30" s="67"/>
       <c r="B30" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="69"/>
-      <c r="D30" s="70"/>
-      <c r="G30" s="75"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="80"/>
+      <c r="G30" s="77"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A31" s="67">
@@ -3798,27 +3798,27 @@
       <c r="B31" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="69"/>
-      <c r="D31" s="70"/>
-      <c r="G31" s="75"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="80"/>
+      <c r="G31" s="77"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A32" s="67"/>
       <c r="B32" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="69"/>
-      <c r="D32" s="70"/>
-      <c r="G32" s="75"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="80"/>
+      <c r="G32" s="77"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A33" s="67"/>
       <c r="B33" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="69"/>
-      <c r="D33" s="70"/>
-      <c r="G33" s="75"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="80"/>
+      <c r="G33" s="77"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A34" s="67">
@@ -3827,27 +3827,27 @@
       <c r="B34" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="69"/>
-      <c r="D34" s="70"/>
-      <c r="G34" s="75"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="80"/>
+      <c r="G34" s="77"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A35" s="67"/>
       <c r="B35" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="69"/>
-      <c r="D35" s="70"/>
-      <c r="G35" s="75"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="80"/>
+      <c r="G35" s="77"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A36" s="67"/>
       <c r="B36" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="69"/>
-      <c r="D36" s="70"/>
-      <c r="G36" s="75"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="80"/>
+      <c r="G36" s="77"/>
     </row>
     <row r="37" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A37" s="6">
@@ -3856,9 +3856,9 @@
       <c r="B37" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="69"/>
-      <c r="D37" s="70"/>
-      <c r="G37" s="75"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="80"/>
+      <c r="G37" s="77"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A38" s="67">
@@ -3867,27 +3867,27 @@
       <c r="B38" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="69"/>
-      <c r="D38" s="70"/>
-      <c r="G38" s="75"/>
+      <c r="C38" s="71"/>
+      <c r="D38" s="80"/>
+      <c r="G38" s="77"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A39" s="67"/>
       <c r="B39" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="69"/>
-      <c r="D39" s="70"/>
-      <c r="G39" s="75"/>
+      <c r="C39" s="71"/>
+      <c r="D39" s="80"/>
+      <c r="G39" s="77"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A40" s="67"/>
       <c r="B40" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="69"/>
-      <c r="D40" s="70"/>
-      <c r="G40" s="75"/>
+      <c r="C40" s="71"/>
+      <c r="D40" s="80"/>
+      <c r="G40" s="77"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A41" s="67">
@@ -3896,27 +3896,27 @@
       <c r="B41" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="69"/>
-      <c r="D41" s="70"/>
-      <c r="G41" s="75"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="80"/>
+      <c r="G41" s="77"/>
     </row>
     <row r="42" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A42" s="67"/>
       <c r="B42" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="69"/>
-      <c r="D42" s="70"/>
-      <c r="G42" s="75"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="80"/>
+      <c r="G42" s="77"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A43" s="67"/>
       <c r="B43" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="69"/>
-      <c r="D43" s="70"/>
-      <c r="G43" s="75"/>
+      <c r="C43" s="71"/>
+      <c r="D43" s="80"/>
+      <c r="G43" s="77"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A44" s="67">
@@ -3925,27 +3925,27 @@
       <c r="B44" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="69"/>
-      <c r="D44" s="70"/>
-      <c r="G44" s="75"/>
+      <c r="C44" s="71"/>
+      <c r="D44" s="80"/>
+      <c r="G44" s="77"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A45" s="67"/>
       <c r="B45" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="69"/>
-      <c r="D45" s="70"/>
-      <c r="G45" s="75"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="80"/>
+      <c r="G45" s="77"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A46" s="67"/>
       <c r="B46" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="69"/>
-      <c r="D46" s="70"/>
-      <c r="G46" s="75"/>
+      <c r="C46" s="71"/>
+      <c r="D46" s="80"/>
+      <c r="G46" s="77"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A47" s="67">
@@ -3954,27 +3954,27 @@
       <c r="B47" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="69"/>
-      <c r="D47" s="70"/>
-      <c r="G47" s="75"/>
+      <c r="C47" s="71"/>
+      <c r="D47" s="80"/>
+      <c r="G47" s="77"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A48" s="67"/>
       <c r="B48" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="69"/>
-      <c r="D48" s="70"/>
-      <c r="G48" s="75"/>
+      <c r="C48" s="71"/>
+      <c r="D48" s="80"/>
+      <c r="G48" s="77"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A49" s="67"/>
       <c r="B49" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="C49" s="69"/>
-      <c r="D49" s="70"/>
-      <c r="G49" s="75"/>
+      <c r="C49" s="71"/>
+      <c r="D49" s="80"/>
+      <c r="G49" s="77"/>
     </row>
     <row r="50" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A50" s="6">
@@ -3983,10 +3983,10 @@
       <c r="B50" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="C50" s="69" t="s">
+      <c r="C50" s="71" t="s">
         <v>157</v>
       </c>
-      <c r="D50" s="70">
+      <c r="D50" s="80">
         <v>1</v>
       </c>
       <c r="E50" s="17"/>
@@ -4001,8 +4001,8 @@
       <c r="B51" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="69"/>
-      <c r="D51" s="70"/>
+      <c r="C51" s="71"/>
+      <c r="D51" s="80"/>
       <c r="G51" s="72"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.6">
@@ -4010,8 +4010,8 @@
       <c r="B52" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="C52" s="69"/>
-      <c r="D52" s="70"/>
+      <c r="C52" s="71"/>
+      <c r="D52" s="80"/>
       <c r="G52" s="72"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.6">
@@ -4019,8 +4019,8 @@
       <c r="B53" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="C53" s="69"/>
-      <c r="D53" s="70"/>
+      <c r="C53" s="71"/>
+      <c r="D53" s="80"/>
       <c r="G53" s="72"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.6">
@@ -4028,8 +4028,8 @@
       <c r="B54" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C54" s="69"/>
-      <c r="D54" s="70"/>
+      <c r="C54" s="71"/>
+      <c r="D54" s="80"/>
       <c r="G54" s="72"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.6">
@@ -4039,8 +4039,8 @@
       <c r="B55" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C55" s="69"/>
-      <c r="D55" s="70"/>
+      <c r="C55" s="71"/>
+      <c r="D55" s="80"/>
       <c r="G55" s="72"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.6">
@@ -4048,8 +4048,8 @@
       <c r="B56" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="C56" s="69"/>
-      <c r="D56" s="70"/>
+      <c r="C56" s="71"/>
+      <c r="D56" s="80"/>
       <c r="G56" s="72"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.6">
@@ -4057,8 +4057,8 @@
       <c r="B57" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="C57" s="69"/>
-      <c r="D57" s="70"/>
+      <c r="C57" s="71"/>
+      <c r="D57" s="80"/>
       <c r="G57" s="72"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.6">
@@ -4068,8 +4068,8 @@
       <c r="B58" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C58" s="69"/>
-      <c r="D58" s="70"/>
+      <c r="C58" s="71"/>
+      <c r="D58" s="80"/>
       <c r="G58" s="72"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.6">
@@ -4077,8 +4077,8 @@
       <c r="B59" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C59" s="69"/>
-      <c r="D59" s="70"/>
+      <c r="C59" s="71"/>
+      <c r="D59" s="80"/>
       <c r="G59" s="72"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.6">
@@ -4086,8 +4086,8 @@
       <c r="B60" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="C60" s="69"/>
-      <c r="D60" s="70"/>
+      <c r="C60" s="71"/>
+      <c r="D60" s="80"/>
       <c r="G60" s="72"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.6">
@@ -4097,8 +4097,8 @@
       <c r="B61" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="C61" s="69"/>
-      <c r="D61" s="70"/>
+      <c r="C61" s="71"/>
+      <c r="D61" s="80"/>
       <c r="G61" s="72"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.6">
@@ -4106,8 +4106,8 @@
       <c r="B62" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="C62" s="69"/>
-      <c r="D62" s="70"/>
+      <c r="C62" s="71"/>
+      <c r="D62" s="80"/>
       <c r="G62" s="72"/>
     </row>
     <row r="63" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
@@ -4115,8 +4115,8 @@
       <c r="B63" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="C63" s="69"/>
-      <c r="D63" s="70"/>
+      <c r="C63" s="71"/>
+      <c r="D63" s="80"/>
       <c r="G63" s="72"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.6">
@@ -4124,8 +4124,8 @@
       <c r="B64" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="C64" s="69"/>
-      <c r="D64" s="70"/>
+      <c r="C64" s="71"/>
+      <c r="D64" s="80"/>
       <c r="G64" s="72"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.6">
@@ -4135,8 +4135,8 @@
       <c r="B65" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="C65" s="69"/>
-      <c r="D65" s="70"/>
+      <c r="C65" s="71"/>
+      <c r="D65" s="80"/>
       <c r="G65" s="72"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.6">
@@ -4146,8 +4146,8 @@
       <c r="B66" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="C66" s="69"/>
-      <c r="D66" s="70"/>
+      <c r="C66" s="71"/>
+      <c r="D66" s="80"/>
       <c r="G66" s="72"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.6">
@@ -4155,8 +4155,8 @@
       <c r="B67" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="C67" s="69"/>
-      <c r="D67" s="70"/>
+      <c r="C67" s="71"/>
+      <c r="D67" s="80"/>
       <c r="G67" s="72"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.6">
@@ -4164,8 +4164,8 @@
       <c r="B68" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C68" s="69"/>
-      <c r="D68" s="70"/>
+      <c r="C68" s="71"/>
+      <c r="D68" s="80"/>
       <c r="G68" s="72"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.6">
@@ -4175,8 +4175,8 @@
       <c r="B69" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C69" s="69"/>
-      <c r="D69" s="70"/>
+      <c r="C69" s="71"/>
+      <c r="D69" s="80"/>
       <c r="G69" s="72"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.6">
@@ -4184,8 +4184,8 @@
       <c r="B70" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C70" s="69"/>
-      <c r="D70" s="70"/>
+      <c r="C70" s="71"/>
+      <c r="D70" s="80"/>
       <c r="G70" s="72"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.6">
@@ -4193,8 +4193,8 @@
       <c r="B71" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="C71" s="69"/>
-      <c r="D71" s="70"/>
+      <c r="C71" s="71"/>
+      <c r="D71" s="80"/>
       <c r="G71" s="72"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.6">
@@ -4204,8 +4204,8 @@
       <c r="B72" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="C72" s="69"/>
-      <c r="D72" s="70"/>
+      <c r="C72" s="71"/>
+      <c r="D72" s="80"/>
       <c r="G72" s="72"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.6">
@@ -4213,8 +4213,8 @@
       <c r="B73" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="C73" s="69"/>
-      <c r="D73" s="70"/>
+      <c r="C73" s="71"/>
+      <c r="D73" s="80"/>
       <c r="G73" s="72"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.6">
@@ -4222,8 +4222,8 @@
       <c r="B74" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="C74" s="69"/>
-      <c r="D74" s="70"/>
+      <c r="C74" s="71"/>
+      <c r="D74" s="80"/>
       <c r="G74" s="72"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.6">
@@ -4233,8 +4233,8 @@
       <c r="B75" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="C75" s="69"/>
-      <c r="D75" s="70"/>
+      <c r="C75" s="71"/>
+      <c r="D75" s="80"/>
       <c r="G75" s="72"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.6">
@@ -4242,8 +4242,8 @@
       <c r="B76" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="C76" s="69"/>
-      <c r="D76" s="70"/>
+      <c r="C76" s="71"/>
+      <c r="D76" s="80"/>
       <c r="G76" s="72"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.6">
@@ -4251,8 +4251,8 @@
       <c r="B77" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="C77" s="69"/>
-      <c r="D77" s="70"/>
+      <c r="C77" s="71"/>
+      <c r="D77" s="80"/>
       <c r="G77" s="72"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.6">
@@ -4262,55 +4262,55 @@
       <c r="B78" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C78" s="69"/>
-      <c r="D78" s="70"/>
+      <c r="C78" s="71"/>
+      <c r="D78" s="80"/>
       <c r="G78" s="72"/>
     </row>
     <row r="79" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A79" s="71">
+      <c r="A79" s="79">
         <v>6.1</v>
       </c>
       <c r="B79" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="C79" s="69"/>
-      <c r="D79" s="70"/>
+      <c r="C79" s="71"/>
+      <c r="D79" s="80"/>
       <c r="G79" s="72"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A80" s="71"/>
+      <c r="A80" s="79"/>
       <c r="B80" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="C80" s="69"/>
-      <c r="D80" s="70"/>
+      <c r="C80" s="71"/>
+      <c r="D80" s="80"/>
       <c r="G80" s="72"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A81" s="71"/>
+      <c r="A81" s="79"/>
       <c r="B81" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="C81" s="69"/>
-      <c r="D81" s="70"/>
+      <c r="C81" s="71"/>
+      <c r="D81" s="80"/>
       <c r="G81" s="72"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A82" s="71"/>
+      <c r="A82" s="79"/>
       <c r="B82" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="C82" s="69"/>
-      <c r="D82" s="70"/>
+      <c r="C82" s="71"/>
+      <c r="D82" s="80"/>
       <c r="G82" s="72"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A83" s="71"/>
+      <c r="A83" s="79"/>
       <c r="B83" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="C83" s="69"/>
-      <c r="D83" s="70"/>
+      <c r="C83" s="71"/>
+      <c r="D83" s="80"/>
       <c r="G83" s="72"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.6">
@@ -4320,8 +4320,8 @@
       <c r="B84" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="C84" s="69"/>
-      <c r="D84" s="70"/>
+      <c r="C84" s="71"/>
+      <c r="D84" s="80"/>
       <c r="G84" s="72"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.6">
@@ -4329,8 +4329,8 @@
       <c r="B85" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C85" s="69"/>
-      <c r="D85" s="70"/>
+      <c r="C85" s="71"/>
+      <c r="D85" s="80"/>
       <c r="G85" s="72"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.6">
@@ -4338,8 +4338,8 @@
       <c r="B86" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="C86" s="69"/>
-      <c r="D86" s="70"/>
+      <c r="C86" s="71"/>
+      <c r="D86" s="80"/>
       <c r="G86" s="72"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.6">
@@ -4347,8 +4347,8 @@
       <c r="B87" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="C87" s="69"/>
-      <c r="D87" s="70"/>
+      <c r="C87" s="71"/>
+      <c r="D87" s="80"/>
       <c r="G87" s="72"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.6">
@@ -4356,8 +4356,8 @@
       <c r="B88" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="C88" s="69"/>
-      <c r="D88" s="70"/>
+      <c r="C88" s="71"/>
+      <c r="D88" s="80"/>
       <c r="G88" s="72"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.6">
@@ -4367,8 +4367,8 @@
       <c r="B89" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="C89" s="69"/>
-      <c r="D89" s="70"/>
+      <c r="C89" s="71"/>
+      <c r="D89" s="80"/>
       <c r="G89" s="72"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.6">
@@ -4376,8 +4376,8 @@
       <c r="B90" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="C90" s="69"/>
-      <c r="D90" s="70"/>
+      <c r="C90" s="71"/>
+      <c r="D90" s="80"/>
       <c r="G90" s="72"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.6">
@@ -4385,8 +4385,8 @@
       <c r="B91" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="C91" s="69"/>
-      <c r="D91" s="70"/>
+      <c r="C91" s="71"/>
+      <c r="D91" s="80"/>
       <c r="G91" s="72"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.6">
@@ -4396,8 +4396,8 @@
       <c r="B92" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="C92" s="69"/>
-      <c r="D92" s="70"/>
+      <c r="C92" s="71"/>
+      <c r="D92" s="80"/>
       <c r="G92" s="72"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.6">
@@ -4405,8 +4405,8 @@
       <c r="B93" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="C93" s="69"/>
-      <c r="D93" s="70"/>
+      <c r="C93" s="71"/>
+      <c r="D93" s="80"/>
       <c r="G93" s="72"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.6">
@@ -4414,8 +4414,8 @@
       <c r="B94" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="C94" s="69"/>
-      <c r="D94" s="70"/>
+      <c r="C94" s="71"/>
+      <c r="D94" s="80"/>
       <c r="G94" s="72"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.6">
@@ -4425,8 +4425,8 @@
       <c r="B95" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="C95" s="69"/>
-      <c r="D95" s="70"/>
+      <c r="C95" s="71"/>
+      <c r="D95" s="80"/>
       <c r="G95" s="72"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.6">
@@ -4434,8 +4434,8 @@
       <c r="B96" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="C96" s="69"/>
-      <c r="D96" s="70"/>
+      <c r="C96" s="71"/>
+      <c r="D96" s="80"/>
       <c r="G96" s="72"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.6">
@@ -4443,8 +4443,8 @@
       <c r="B97" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="C97" s="69"/>
-      <c r="D97" s="70"/>
+      <c r="C97" s="71"/>
+      <c r="D97" s="80"/>
       <c r="G97" s="72"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.6">
@@ -4452,8 +4452,8 @@
       <c r="B98" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="C98" s="69"/>
-      <c r="D98" s="70"/>
+      <c r="C98" s="71"/>
+      <c r="D98" s="80"/>
       <c r="G98" s="72"/>
     </row>
     <row r="99" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
@@ -4463,132 +4463,132 @@
       <c r="B99" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C99" s="73" t="s">
+      <c r="C99" s="74" t="s">
         <v>159</v>
       </c>
-      <c r="D99" s="78">
+      <c r="D99" s="68">
         <v>1</v>
       </c>
       <c r="E99" s="17"/>
-      <c r="G99" s="76" t="s">
+      <c r="G99" s="70" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A100" s="77">
+      <c r="A100" s="78">
         <v>7.1</v>
       </c>
       <c r="B100" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="C100" s="73"/>
-      <c r="D100" s="78"/>
-      <c r="G100" s="76"/>
+      <c r="C100" s="74"/>
+      <c r="D100" s="68"/>
+      <c r="G100" s="70"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A101" s="77"/>
+      <c r="A101" s="78"/>
       <c r="B101" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="C101" s="73"/>
-      <c r="D101" s="78"/>
-      <c r="G101" s="76"/>
+      <c r="C101" s="74"/>
+      <c r="D101" s="68"/>
+      <c r="G101" s="70"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A102" s="77"/>
+      <c r="A102" s="78"/>
       <c r="B102" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="C102" s="73"/>
-      <c r="D102" s="78"/>
-      <c r="G102" s="76"/>
+      <c r="C102" s="74"/>
+      <c r="D102" s="68"/>
+      <c r="G102" s="70"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A103" s="77">
+      <c r="A103" s="78">
         <v>7.2</v>
       </c>
       <c r="B103" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="C103" s="73"/>
-      <c r="D103" s="78"/>
-      <c r="G103" s="76"/>
+      <c r="C103" s="74"/>
+      <c r="D103" s="68"/>
+      <c r="G103" s="70"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A104" s="77"/>
+      <c r="A104" s="78"/>
       <c r="B104" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="C104" s="73"/>
-      <c r="D104" s="78"/>
-      <c r="G104" s="76"/>
+      <c r="C104" s="74"/>
+      <c r="D104" s="68"/>
+      <c r="G104" s="70"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A105" s="77"/>
+      <c r="A105" s="78"/>
       <c r="B105" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="C105" s="73"/>
-      <c r="D105" s="78"/>
-      <c r="G105" s="76"/>
+      <c r="C105" s="74"/>
+      <c r="D105" s="68"/>
+      <c r="G105" s="70"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A106" s="77">
+      <c r="A106" s="78">
         <v>7.3</v>
       </c>
       <c r="B106" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="C106" s="73"/>
-      <c r="D106" s="78"/>
-      <c r="G106" s="76"/>
+      <c r="C106" s="74"/>
+      <c r="D106" s="68"/>
+      <c r="G106" s="70"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A107" s="77"/>
+      <c r="A107" s="78"/>
       <c r="B107" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="C107" s="73"/>
-      <c r="D107" s="78"/>
-      <c r="G107" s="76"/>
+      <c r="C107" s="74"/>
+      <c r="D107" s="68"/>
+      <c r="G107" s="70"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A108" s="77"/>
+      <c r="A108" s="78"/>
       <c r="B108" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C108" s="73"/>
-      <c r="D108" s="78"/>
-      <c r="G108" s="76"/>
+      <c r="C108" s="74"/>
+      <c r="D108" s="68"/>
+      <c r="G108" s="70"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A109" s="77">
+      <c r="A109" s="78">
         <v>7.4</v>
       </c>
       <c r="B109" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="C109" s="73"/>
-      <c r="D109" s="78"/>
-      <c r="G109" s="76"/>
+      <c r="C109" s="74"/>
+      <c r="D109" s="68"/>
+      <c r="G109" s="70"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A110" s="77"/>
+      <c r="A110" s="78"/>
       <c r="B110" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="C110" s="73"/>
-      <c r="D110" s="78"/>
-      <c r="G110" s="76"/>
+      <c r="C110" s="74"/>
+      <c r="D110" s="68"/>
+      <c r="G110" s="70"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A111" s="77"/>
+      <c r="A111" s="78"/>
       <c r="B111" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="C111" s="73"/>
-      <c r="D111" s="78"/>
-      <c r="G111" s="76"/>
+      <c r="C111" s="74"/>
+      <c r="D111" s="68"/>
+      <c r="G111" s="70"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A112" s="5">
@@ -4597,9 +4597,9 @@
       <c r="B112" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C112" s="73"/>
-      <c r="D112" s="78"/>
-      <c r="G112" s="76"/>
+      <c r="C112" s="74"/>
+      <c r="D112" s="68"/>
+      <c r="G112" s="70"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A113" s="33">
@@ -4608,101 +4608,101 @@
       <c r="B113" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="C113" s="73"/>
-      <c r="D113" s="78"/>
-      <c r="G113" s="76"/>
+      <c r="C113" s="74"/>
+      <c r="D113" s="68"/>
+      <c r="G113" s="70"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A114" s="77">
+      <c r="A114" s="78">
         <v>8.1</v>
       </c>
       <c r="B114" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="C114" s="73"/>
-      <c r="D114" s="78"/>
-      <c r="G114" s="76"/>
+      <c r="C114" s="74"/>
+      <c r="D114" s="68"/>
+      <c r="G114" s="70"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A115" s="77"/>
+      <c r="A115" s="78"/>
       <c r="B115" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="C115" s="73"/>
-      <c r="D115" s="78"/>
-      <c r="G115" s="76"/>
+      <c r="C115" s="74"/>
+      <c r="D115" s="68"/>
+      <c r="G115" s="70"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A116" s="77"/>
+      <c r="A116" s="78"/>
       <c r="B116" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="C116" s="73"/>
-      <c r="D116" s="78"/>
-      <c r="G116" s="76"/>
+      <c r="C116" s="74"/>
+      <c r="D116" s="68"/>
+      <c r="G116" s="70"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A117" s="77"/>
+      <c r="A117" s="78"/>
       <c r="B117" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="C117" s="73"/>
-      <c r="D117" s="78"/>
-      <c r="G117" s="76"/>
+      <c r="C117" s="74"/>
+      <c r="D117" s="68"/>
+      <c r="G117" s="70"/>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A118" s="77"/>
+      <c r="A118" s="78"/>
       <c r="B118" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="C118" s="73"/>
-      <c r="D118" s="78"/>
-      <c r="G118" s="76"/>
+      <c r="C118" s="74"/>
+      <c r="D118" s="68"/>
+      <c r="G118" s="70"/>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A119" s="77"/>
+      <c r="A119" s="78"/>
       <c r="B119" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="C119" s="73"/>
-      <c r="D119" s="78"/>
-      <c r="G119" s="76"/>
+      <c r="C119" s="74"/>
+      <c r="D119" s="68"/>
+      <c r="G119" s="70"/>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A120" s="77"/>
+      <c r="A120" s="78"/>
       <c r="B120" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="C120" s="73"/>
-      <c r="D120" s="78"/>
-      <c r="G120" s="76"/>
+      <c r="C120" s="74"/>
+      <c r="D120" s="68"/>
+      <c r="G120" s="70"/>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A121" s="67"/>
       <c r="B121" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="C121" s="73"/>
-      <c r="D121" s="78"/>
-      <c r="G121" s="76"/>
+      <c r="C121" s="74"/>
+      <c r="D121" s="68"/>
+      <c r="G121" s="70"/>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A122" s="67"/>
       <c r="B122" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="C122" s="73"/>
-      <c r="D122" s="78"/>
-      <c r="G122" s="76"/>
+      <c r="C122" s="74"/>
+      <c r="D122" s="68"/>
+      <c r="G122" s="70"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A123" s="67"/>
       <c r="B123" s="36" t="s">
         <v>152</v>
       </c>
-      <c r="C123" s="73"/>
-      <c r="D123" s="78"/>
-      <c r="G123" s="76"/>
+      <c r="C123" s="74"/>
+      <c r="D123" s="68"/>
+      <c r="G123" s="70"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A124" s="32">
@@ -4711,61 +4711,61 @@
       <c r="B124" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="C124" s="73" t="s">
+      <c r="C124" s="74" t="s">
         <v>168</v>
       </c>
-      <c r="D124" s="78">
+      <c r="D124" s="68">
         <v>0.75</v>
       </c>
       <c r="E124" s="17"/>
-      <c r="G124" s="76"/>
+      <c r="G124" s="70"/>
     </row>
     <row r="125" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A125" s="81">
+      <c r="A125" s="69">
         <v>9.1</v>
       </c>
       <c r="B125" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="C125" s="73"/>
-      <c r="D125" s="78"/>
-      <c r="G125" s="76"/>
+      <c r="C125" s="74"/>
+      <c r="D125" s="68"/>
+      <c r="G125" s="70"/>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A126" s="81"/>
+      <c r="A126" s="69"/>
       <c r="B126" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="C126" s="73"/>
-      <c r="D126" s="78"/>
-      <c r="G126" s="76"/>
+      <c r="C126" s="74"/>
+      <c r="D126" s="68"/>
+      <c r="G126" s="70"/>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A127" s="81"/>
+      <c r="A127" s="69"/>
       <c r="B127" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="C127" s="73"/>
-      <c r="D127" s="78"/>
-      <c r="G127" s="76"/>
+      <c r="C127" s="74"/>
+      <c r="D127" s="68"/>
+      <c r="G127" s="70"/>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A128" s="81"/>
+      <c r="A128" s="69"/>
       <c r="B128" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="C128" s="73"/>
-      <c r="D128" s="78"/>
-      <c r="G128" s="76"/>
+      <c r="C128" s="74"/>
+      <c r="D128" s="68"/>
+      <c r="G128" s="70"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A129" s="81"/>
+      <c r="A129" s="69"/>
       <c r="B129" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="C129" s="73"/>
-      <c r="D129" s="78"/>
-      <c r="G129" s="76"/>
+      <c r="C129" s="74"/>
+      <c r="D129" s="68"/>
+      <c r="G129" s="70"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A130" s="67">
@@ -4774,36 +4774,36 @@
       <c r="B130" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="C130" s="73"/>
-      <c r="D130" s="78"/>
-      <c r="G130" s="76"/>
+      <c r="C130" s="74"/>
+      <c r="D130" s="68"/>
+      <c r="G130" s="70"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A131" s="67"/>
       <c r="B131" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="C131" s="73"/>
-      <c r="D131" s="78"/>
-      <c r="G131" s="76"/>
+      <c r="C131" s="74"/>
+      <c r="D131" s="68"/>
+      <c r="G131" s="70"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A132" s="67"/>
       <c r="B132" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="C132" s="73"/>
-      <c r="D132" s="78"/>
-      <c r="G132" s="76"/>
+      <c r="C132" s="74"/>
+      <c r="D132" s="68"/>
+      <c r="G132" s="70"/>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A133" s="67"/>
       <c r="B133" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="C133" s="73"/>
-      <c r="D133" s="78"/>
-      <c r="G133" s="76"/>
+      <c r="C133" s="74"/>
+      <c r="D133" s="68"/>
+      <c r="G133" s="70"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A134" s="67">
@@ -4812,36 +4812,36 @@
       <c r="B134" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="C134" s="73"/>
-      <c r="D134" s="78"/>
-      <c r="G134" s="76"/>
+      <c r="C134" s="74"/>
+      <c r="D134" s="68"/>
+      <c r="G134" s="70"/>
     </row>
     <row r="135" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A135" s="67"/>
       <c r="B135" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="C135" s="73"/>
-      <c r="D135" s="78"/>
-      <c r="G135" s="76"/>
+      <c r="C135" s="74"/>
+      <c r="D135" s="68"/>
+      <c r="G135" s="70"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A136" s="67"/>
       <c r="B136" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C136" s="73"/>
-      <c r="D136" s="78"/>
-      <c r="G136" s="76"/>
+      <c r="C136" s="74"/>
+      <c r="D136" s="68"/>
+      <c r="G136" s="70"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A137" s="67"/>
       <c r="B137" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="C137" s="73"/>
-      <c r="D137" s="78"/>
-      <c r="G137" s="76"/>
+      <c r="C137" s="74"/>
+      <c r="D137" s="68"/>
+      <c r="G137" s="70"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A138" s="67">
@@ -4850,36 +4850,36 @@
       <c r="B138" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="C138" s="73"/>
-      <c r="D138" s="78"/>
-      <c r="G138" s="76"/>
+      <c r="C138" s="74"/>
+      <c r="D138" s="68"/>
+      <c r="G138" s="70"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A139" s="67"/>
       <c r="B139" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="C139" s="73"/>
-      <c r="D139" s="78"/>
-      <c r="G139" s="76"/>
+      <c r="C139" s="74"/>
+      <c r="D139" s="68"/>
+      <c r="G139" s="70"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A140" s="67"/>
       <c r="B140" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="C140" s="73"/>
-      <c r="D140" s="78"/>
-      <c r="G140" s="76"/>
+      <c r="C140" s="74"/>
+      <c r="D140" s="68"/>
+      <c r="G140" s="70"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A141" s="67"/>
       <c r="B141" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="C141" s="73"/>
-      <c r="D141" s="78"/>
-      <c r="G141" s="76"/>
+      <c r="C141" s="74"/>
+      <c r="D141" s="68"/>
+      <c r="G141" s="70"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A142" s="6">
@@ -4888,14 +4888,14 @@
       <c r="B142" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="C142" s="69" t="s">
+      <c r="C142" s="71" t="s">
         <v>169</v>
       </c>
-      <c r="D142" s="78">
+      <c r="D142" s="68">
         <v>1.75</v>
       </c>
       <c r="E142" s="17"/>
-      <c r="G142" s="76"/>
+      <c r="G142" s="70"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A143" s="5">
@@ -4904,9 +4904,9 @@
       <c r="B143" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="C143" s="69"/>
-      <c r="D143" s="78"/>
-      <c r="G143" s="76"/>
+      <c r="C143" s="71"/>
+      <c r="D143" s="68"/>
+      <c r="G143" s="70"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A144" s="6">
@@ -4915,10 +4915,10 @@
       <c r="B144" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="C144" s="73" t="s">
+      <c r="C144" s="74" t="s">
         <v>170</v>
       </c>
-      <c r="D144" s="78">
+      <c r="D144" s="68">
         <v>0.5</v>
       </c>
       <c r="E144" s="17"/>
@@ -4931,8 +4931,8 @@
       <c r="B145" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C145" s="80"/>
-      <c r="D145" s="78"/>
+      <c r="C145" s="75"/>
+      <c r="D145" s="68"/>
       <c r="G145" s="72"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.6">
@@ -4940,8 +4940,8 @@
       <c r="B146" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C146" s="80"/>
-      <c r="D146" s="78"/>
+      <c r="C146" s="75"/>
+      <c r="D146" s="68"/>
       <c r="G146" s="72"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.6">
@@ -4949,8 +4949,8 @@
       <c r="B147" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C147" s="80"/>
-      <c r="D147" s="78"/>
+      <c r="C147" s="75"/>
+      <c r="D147" s="68"/>
       <c r="G147" s="72"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.6">
@@ -4960,8 +4960,8 @@
       <c r="B148" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C148" s="80"/>
-      <c r="D148" s="78"/>
+      <c r="C148" s="75"/>
+      <c r="D148" s="68"/>
       <c r="G148" s="72"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.6">
@@ -4969,8 +4969,8 @@
       <c r="B149" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C149" s="80"/>
-      <c r="D149" s="78"/>
+      <c r="C149" s="75"/>
+      <c r="D149" s="68"/>
       <c r="G149" s="72"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.6">
@@ -4978,133 +4978,143 @@
       <c r="B150" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C150" s="80"/>
-      <c r="D150" s="78"/>
+      <c r="C150" s="75"/>
+      <c r="D150" s="68"/>
       <c r="G150" s="72"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A151" s="79">
+      <c r="A151" s="73">
         <v>11.3</v>
       </c>
       <c r="B151" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="C151" s="80"/>
-      <c r="D151" s="78"/>
+      <c r="C151" s="75"/>
+      <c r="D151" s="68"/>
       <c r="G151" s="72"/>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A152" s="79"/>
+      <c r="A152" s="73"/>
       <c r="B152" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C152" s="80"/>
-      <c r="D152" s="78"/>
+      <c r="C152" s="75"/>
+      <c r="D152" s="68"/>
       <c r="G152" s="72"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A153" s="79"/>
+      <c r="A153" s="73"/>
       <c r="B153" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C153" s="80"/>
-      <c r="D153" s="78"/>
+      <c r="C153" s="75"/>
+      <c r="D153" s="68"/>
       <c r="G153" s="72"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A154" s="79"/>
+      <c r="A154" s="73"/>
       <c r="B154" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C154" s="80"/>
-      <c r="D154" s="78"/>
+      <c r="C154" s="75"/>
+      <c r="D154" s="68"/>
       <c r="G154" s="72"/>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A155" s="79">
+      <c r="A155" s="73">
         <v>11.4</v>
       </c>
       <c r="B155" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="C155" s="80"/>
-      <c r="D155" s="78"/>
+      <c r="C155" s="75"/>
+      <c r="D155" s="68"/>
       <c r="G155" s="72"/>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A156" s="79"/>
+      <c r="A156" s="73"/>
       <c r="B156" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="C156" s="80"/>
-      <c r="D156" s="78"/>
+      <c r="C156" s="75"/>
+      <c r="D156" s="68"/>
       <c r="G156" s="72"/>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A157" s="79"/>
+      <c r="A157" s="73"/>
       <c r="B157" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="C157" s="80"/>
-      <c r="D157" s="78"/>
+      <c r="C157" s="75"/>
+      <c r="D157" s="68"/>
       <c r="G157" s="72"/>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A158" s="79">
+      <c r="A158" s="73">
         <v>11.5</v>
       </c>
       <c r="B158" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="C158" s="80"/>
-      <c r="D158" s="78"/>
+      <c r="C158" s="75"/>
+      <c r="D158" s="68"/>
       <c r="G158" s="72"/>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A159" s="79"/>
+      <c r="A159" s="73"/>
       <c r="B159" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="C159" s="80"/>
-      <c r="D159" s="78"/>
+      <c r="C159" s="75"/>
+      <c r="D159" s="68"/>
       <c r="G159" s="72"/>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A160" s="79"/>
+      <c r="A160" s="73"/>
       <c r="B160" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="C160" s="80"/>
-      <c r="D160" s="78"/>
+      <c r="C160" s="75"/>
+      <c r="D160" s="68"/>
       <c r="G160" s="72"/>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A161" s="79"/>
+      <c r="A161" s="73"/>
       <c r="B161" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="C161" s="80"/>
-      <c r="D161" s="78"/>
+      <c r="C161" s="75"/>
+      <c r="D161" s="68"/>
       <c r="G161" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="A130:A133"/>
-    <mergeCell ref="A134:A137"/>
-    <mergeCell ref="A138:A141"/>
-    <mergeCell ref="D124:D141"/>
-    <mergeCell ref="A125:A129"/>
-    <mergeCell ref="G142:G143"/>
-    <mergeCell ref="C142:C143"/>
-    <mergeCell ref="D142:D143"/>
-    <mergeCell ref="A145:A147"/>
-    <mergeCell ref="G144:G161"/>
-    <mergeCell ref="D144:D161"/>
-    <mergeCell ref="A148:A150"/>
-    <mergeCell ref="A151:A154"/>
-    <mergeCell ref="A155:A157"/>
-    <mergeCell ref="A158:A161"/>
-    <mergeCell ref="C144:C161"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="C5:C49"/>
+    <mergeCell ref="D5:D49"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="C50:C98"/>
+    <mergeCell ref="D50:D98"/>
+    <mergeCell ref="G50:G98"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="A95:A98"/>
     <mergeCell ref="C99:C123"/>
     <mergeCell ref="G5:G49"/>
     <mergeCell ref="G99:G141"/>
@@ -5121,32 +5131,22 @@
     <mergeCell ref="A89:A91"/>
     <mergeCell ref="A92:A94"/>
     <mergeCell ref="D99:D123"/>
-    <mergeCell ref="C50:C98"/>
-    <mergeCell ref="D50:D98"/>
-    <mergeCell ref="G50:G98"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="C5:C49"/>
-    <mergeCell ref="D5:D49"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="G142:G143"/>
+    <mergeCell ref="C142:C143"/>
+    <mergeCell ref="D142:D143"/>
+    <mergeCell ref="A145:A147"/>
+    <mergeCell ref="G144:G161"/>
+    <mergeCell ref="D144:D161"/>
+    <mergeCell ref="A148:A150"/>
+    <mergeCell ref="A151:A154"/>
+    <mergeCell ref="A155:A157"/>
+    <mergeCell ref="A158:A161"/>
+    <mergeCell ref="C144:C161"/>
+    <mergeCell ref="A130:A133"/>
+    <mergeCell ref="A134:A137"/>
+    <mergeCell ref="A138:A141"/>
+    <mergeCell ref="D124:D141"/>
+    <mergeCell ref="A125:A129"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Generics & Dynamic Polymorphiism _C#
</commit_message>
<xml_diff>
--- a/CP_Platform_Solution_.Net_v1.4-Phase1.xlsx
+++ b/CP_Platform_Solution_.Net_v1.4-Phase1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anami\Wipro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D853E5-BBA3-496A-9C75-793EC3F22448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7375569-4D0D-4598-BA67-4551713ADF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" activeTab="2" xr2:uid="{A334C00E-DF14-8E42-AC33-43AB2B07B0C8}"/>
   </bookViews>
@@ -2067,7 +2067,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2177,21 +2177,81 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="7"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2201,110 +2261,53 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2722,16 +2725,16 @@
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="62" t="s">
         <v>171</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A2" s="18" t="s">
@@ -2750,13 +2753,13 @@
       <c r="A4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
       <c r="G4" s="19" t="s">
         <v>6</v>
       </c>
@@ -2771,187 +2774,187 @@
       <c r="A5" s="20">
         <v>1</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="48" t="s">
         <v>172</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="44" t="s">
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="64" t="s">
         <v>173</v>
       </c>
-      <c r="H5" s="44" t="s">
+      <c r="H5" s="64" t="s">
         <v>174</v>
       </c>
-      <c r="I5" s="47">
+      <c r="I5" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A6" s="50">
+      <c r="A6" s="39">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="48"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="56"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A7" s="51"/>
-      <c r="B7" s="57" t="s">
+      <c r="A7" s="40"/>
+      <c r="B7" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="48"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="56"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A8" s="51"/>
-      <c r="B8" s="57" t="s">
+      <c r="A8" s="40"/>
+      <c r="B8" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="48"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="56"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A9" s="51"/>
-      <c r="B9" s="57" t="s">
+      <c r="A9" s="40"/>
+      <c r="B9" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="48"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="56"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A10" s="51"/>
-      <c r="B10" s="57" t="s">
+      <c r="A10" s="40"/>
+      <c r="B10" s="45" t="s">
         <v>179</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="48"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="56"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A11" s="51"/>
-      <c r="B11" s="60" t="s">
+      <c r="A11" s="40"/>
+      <c r="B11" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="48"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="56"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A12" s="55"/>
-      <c r="B12" s="60" t="s">
+      <c r="A12" s="41"/>
+      <c r="B12" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="48"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="56"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A13" s="50">
+      <c r="A13" s="39">
         <v>1.2</v>
       </c>
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="48"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="56"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A14" s="51"/>
-      <c r="B14" s="57" t="s">
+      <c r="A14" s="40"/>
+      <c r="B14" s="45" t="s">
         <v>183</v>
       </c>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="48"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="56"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A15" s="51"/>
-      <c r="B15" s="57" t="s">
+      <c r="A15" s="40"/>
+      <c r="B15" s="45" t="s">
         <v>184</v>
       </c>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="48"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="56"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A16" s="55"/>
-      <c r="B16" s="57" t="s">
+      <c r="A16" s="41"/>
+      <c r="B16" s="45" t="s">
         <v>185</v>
       </c>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="48"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="56"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A17" s="50">
+      <c r="A17" s="39">
         <v>1.3</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="58" t="s">
         <v>186</v>
       </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="48"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="56"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A18" s="51"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="25" t="s">
         <v>187</v>
       </c>
@@ -2959,12 +2962,12 @@
       <c r="D18" s="26"/>
       <c r="E18" s="26"/>
       <c r="F18" s="27"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="48"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="56"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A19" s="51"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="25" t="s">
         <v>188</v>
       </c>
@@ -2972,318 +2975,318 @@
       <c r="D19" s="26"/>
       <c r="E19" s="26"/>
       <c r="F19" s="27"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="48"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="56"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A20" s="50">
+      <c r="A20" s="39">
         <v>1.4</v>
       </c>
-      <c r="B20" s="56" t="s">
+      <c r="B20" s="42" t="s">
         <v>189</v>
       </c>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="48"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="56"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A21" s="51"/>
-      <c r="B21" s="57" t="s">
+      <c r="A21" s="40"/>
+      <c r="B21" s="45" t="s">
         <v>190</v>
       </c>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="48"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="56"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A22" s="51"/>
-      <c r="B22" s="57" t="s">
+      <c r="A22" s="40"/>
+      <c r="B22" s="45" t="s">
         <v>191</v>
       </c>
-      <c r="C22" s="58"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="58"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="48"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="56"/>
     </row>
     <row r="23" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A23" s="55"/>
-      <c r="B23" s="57" t="s">
+      <c r="A23" s="41"/>
+      <c r="B23" s="45" t="s">
         <v>192</v>
       </c>
-      <c r="C23" s="58"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="58"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="48"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="65"/>
+      <c r="I23" s="56"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A24" s="50">
+      <c r="A24" s="39">
         <v>1.5</v>
       </c>
-      <c r="B24" s="56" t="s">
+      <c r="B24" s="42" t="s">
         <v>193</v>
       </c>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="48"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="56"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A25" s="51"/>
-      <c r="B25" s="57" t="s">
+      <c r="A25" s="40"/>
+      <c r="B25" s="45" t="s">
         <v>194</v>
       </c>
-      <c r="C25" s="58"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="48"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="56"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A26" s="51"/>
-      <c r="B26" s="57" t="s">
+      <c r="A26" s="40"/>
+      <c r="B26" s="45" t="s">
         <v>195</v>
       </c>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="48"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="56"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A27" s="55"/>
-      <c r="B27" s="57" t="s">
+      <c r="A27" s="41"/>
+      <c r="B27" s="45" t="s">
         <v>196</v>
       </c>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="46"/>
-      <c r="I27" s="49"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="66"/>
+      <c r="I27" s="57"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A28" s="20">
         <v>2</v>
       </c>
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="63" t="s">
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="51" t="s">
         <v>198</v>
       </c>
-      <c r="H28" s="66" t="s">
+      <c r="H28" s="54" t="s">
         <v>199</v>
       </c>
-      <c r="I28" s="47">
+      <c r="I28" s="55">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A29" s="50">
+      <c r="A29" s="39">
         <v>2.1</v>
       </c>
-      <c r="B29" s="56" t="s">
+      <c r="B29" s="42" t="s">
         <v>200</v>
       </c>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="64"/>
-      <c r="I29" s="48"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="56"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A30" s="51"/>
-      <c r="B30" s="57" t="s">
+      <c r="A30" s="40"/>
+      <c r="B30" s="45" t="s">
         <v>201</v>
       </c>
-      <c r="C30" s="58"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="64"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="48"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="56"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A31" s="51"/>
-      <c r="B31" s="57" t="s">
+      <c r="A31" s="40"/>
+      <c r="B31" s="45" t="s">
         <v>202</v>
       </c>
-      <c r="C31" s="58"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="64"/>
-      <c r="H31" s="64"/>
-      <c r="I31" s="48"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="56"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A32" s="55"/>
-      <c r="B32" s="57" t="s">
+      <c r="A32" s="41"/>
+      <c r="B32" s="45" t="s">
         <v>203</v>
       </c>
-      <c r="C32" s="58"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="58"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="64"/>
-      <c r="I32" s="48"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="56"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A33" s="50">
+      <c r="A33" s="39">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B33" s="56" t="s">
+      <c r="B33" s="42" t="s">
         <v>204</v>
       </c>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="64"/>
-      <c r="H33" s="64"/>
-      <c r="I33" s="48"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="52"/>
+      <c r="I33" s="56"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A34" s="51"/>
-      <c r="B34" s="57" t="s">
+      <c r="A34" s="40"/>
+      <c r="B34" s="45" t="s">
         <v>205</v>
       </c>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="59"/>
-      <c r="G34" s="64"/>
-      <c r="H34" s="64"/>
-      <c r="I34" s="48"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="52"/>
+      <c r="I34" s="56"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A35" s="51"/>
-      <c r="B35" s="57" t="s">
+      <c r="A35" s="40"/>
+      <c r="B35" s="45" t="s">
         <v>206</v>
       </c>
-      <c r="C35" s="58"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="58"/>
-      <c r="F35" s="59"/>
-      <c r="G35" s="64"/>
-      <c r="H35" s="64"/>
-      <c r="I35" s="48"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="46"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="52"/>
+      <c r="I35" s="56"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A36" s="55"/>
-      <c r="B36" s="57" t="s">
+      <c r="A36" s="41"/>
+      <c r="B36" s="45" t="s">
         <v>207</v>
       </c>
-      <c r="C36" s="58"/>
-      <c r="D36" s="58"/>
-      <c r="E36" s="58"/>
-      <c r="F36" s="59"/>
-      <c r="G36" s="64"/>
-      <c r="H36" s="64"/>
-      <c r="I36" s="48"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="52"/>
+      <c r="I36" s="56"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A37" s="50">
+      <c r="A37" s="39">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B37" s="56" t="s">
+      <c r="B37" s="42" t="s">
         <v>208</v>
       </c>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="64"/>
-      <c r="H37" s="64"/>
-      <c r="I37" s="48"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="56"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A38" s="51"/>
-      <c r="B38" s="57" t="s">
+      <c r="A38" s="40"/>
+      <c r="B38" s="45" t="s">
         <v>209</v>
       </c>
-      <c r="C38" s="58"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="58"/>
-      <c r="F38" s="59"/>
-      <c r="G38" s="64"/>
-      <c r="H38" s="64"/>
-      <c r="I38" s="48"/>
+      <c r="C38" s="46"/>
+      <c r="D38" s="46"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="52"/>
+      <c r="H38" s="52"/>
+      <c r="I38" s="56"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A39" s="51"/>
-      <c r="B39" s="57" t="s">
+      <c r="A39" s="40"/>
+      <c r="B39" s="45" t="s">
         <v>210</v>
       </c>
-      <c r="C39" s="58"/>
-      <c r="D39" s="58"/>
-      <c r="E39" s="58"/>
-      <c r="F39" s="59"/>
-      <c r="G39" s="64"/>
-      <c r="H39" s="64"/>
-      <c r="I39" s="48"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="52"/>
+      <c r="I39" s="56"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A40" s="55"/>
-      <c r="B40" s="57" t="s">
+      <c r="A40" s="41"/>
+      <c r="B40" s="45" t="s">
         <v>211</v>
       </c>
-      <c r="C40" s="58"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="58"/>
-      <c r="F40" s="59"/>
-      <c r="G40" s="64"/>
-      <c r="H40" s="64"/>
-      <c r="I40" s="48"/>
+      <c r="C40" s="46"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="52"/>
+      <c r="H40" s="52"/>
+      <c r="I40" s="56"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A41" s="50">
+      <c r="A41" s="39">
         <v>2.4</v>
       </c>
-      <c r="B41" s="56" t="s">
+      <c r="B41" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="C41" s="53"/>
-      <c r="D41" s="53"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="54"/>
-      <c r="G41" s="64"/>
-      <c r="H41" s="64"/>
-      <c r="I41" s="48"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="44"/>
+      <c r="G41" s="52"/>
+      <c r="H41" s="52"/>
+      <c r="I41" s="56"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A42" s="51"/>
+      <c r="A42" s="40"/>
       <c r="B42" s="25" t="s">
         <v>213</v>
       </c>
@@ -3291,12 +3294,12 @@
       <c r="D42" s="26"/>
       <c r="E42" s="26"/>
       <c r="F42" s="27"/>
-      <c r="G42" s="64"/>
-      <c r="H42" s="64"/>
-      <c r="I42" s="48"/>
+      <c r="G42" s="52"/>
+      <c r="H42" s="52"/>
+      <c r="I42" s="56"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A43" s="55"/>
+      <c r="A43" s="41"/>
       <c r="B43" s="25" t="s">
         <v>214</v>
       </c>
@@ -3304,27 +3307,27 @@
       <c r="D43" s="26"/>
       <c r="E43" s="26"/>
       <c r="F43" s="27"/>
-      <c r="G43" s="64"/>
-      <c r="H43" s="64"/>
-      <c r="I43" s="48"/>
+      <c r="G43" s="52"/>
+      <c r="H43" s="52"/>
+      <c r="I43" s="56"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A44" s="50">
+      <c r="A44" s="39">
         <v>2.5</v>
       </c>
-      <c r="B44" s="56" t="s">
+      <c r="B44" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="C44" s="53"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="53"/>
-      <c r="F44" s="54"/>
-      <c r="G44" s="64"/>
-      <c r="H44" s="64"/>
-      <c r="I44" s="48"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="43"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="56"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A45" s="51"/>
+      <c r="A45" s="40"/>
       <c r="B45" s="25" t="s">
         <v>216</v>
       </c>
@@ -3332,12 +3335,12 @@
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="27"/>
-      <c r="G45" s="64"/>
-      <c r="H45" s="64"/>
-      <c r="I45" s="48"/>
+      <c r="G45" s="52"/>
+      <c r="H45" s="52"/>
+      <c r="I45" s="56"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A46" s="55"/>
+      <c r="A46" s="41"/>
       <c r="B46" s="25" t="s">
         <v>217</v>
       </c>
@@ -3345,78 +3348,97 @@
       <c r="D46" s="26"/>
       <c r="E46" s="26"/>
       <c r="F46" s="27"/>
-      <c r="G46" s="64"/>
-      <c r="H46" s="64"/>
-      <c r="I46" s="48"/>
+      <c r="G46" s="52"/>
+      <c r="H46" s="52"/>
+      <c r="I46" s="56"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A47" s="50">
+      <c r="A47" s="39">
         <v>2.6</v>
       </c>
-      <c r="B47" s="56" t="s">
+      <c r="B47" s="42" t="s">
         <v>218</v>
       </c>
-      <c r="C47" s="53"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="53"/>
-      <c r="F47" s="54"/>
-      <c r="G47" s="64"/>
-      <c r="H47" s="64"/>
-      <c r="I47" s="48"/>
+      <c r="C47" s="43"/>
+      <c r="D47" s="43"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="52"/>
+      <c r="H47" s="52"/>
+      <c r="I47" s="56"/>
     </row>
     <row r="48" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A48" s="51"/>
-      <c r="B48" s="57" t="s">
+      <c r="A48" s="40"/>
+      <c r="B48" s="45" t="s">
         <v>219</v>
       </c>
-      <c r="C48" s="58"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="58"/>
-      <c r="F48" s="59"/>
-      <c r="G48" s="64"/>
-      <c r="H48" s="64"/>
-      <c r="I48" s="48"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="52"/>
+      <c r="H48" s="52"/>
+      <c r="I48" s="56"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A49" s="51"/>
-      <c r="B49" s="57" t="s">
+      <c r="A49" s="40"/>
+      <c r="B49" s="45" t="s">
         <v>220</v>
       </c>
-      <c r="C49" s="58"/>
-      <c r="D49" s="58"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="59"/>
-      <c r="G49" s="64"/>
-      <c r="H49" s="64"/>
-      <c r="I49" s="48"/>
+      <c r="C49" s="46"/>
+      <c r="D49" s="46"/>
+      <c r="E49" s="46"/>
+      <c r="F49" s="47"/>
+      <c r="G49" s="52"/>
+      <c r="H49" s="52"/>
+      <c r="I49" s="56"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A50" s="55"/>
-      <c r="B50" s="57" t="s">
+      <c r="A50" s="41"/>
+      <c r="B50" s="45" t="s">
         <v>221</v>
       </c>
-      <c r="C50" s="58"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="58"/>
-      <c r="F50" s="59"/>
-      <c r="G50" s="65"/>
-      <c r="H50" s="65"/>
-      <c r="I50" s="49"/>
+      <c r="C50" s="46"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="47"/>
+      <c r="G50" s="53"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="G5:G27"/>
+    <mergeCell ref="H5:H27"/>
+    <mergeCell ref="I5:I27"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
     <mergeCell ref="B28:F28"/>
     <mergeCell ref="G28:G50"/>
     <mergeCell ref="H28:H50"/>
@@ -3433,37 +3455,18 @@
     <mergeCell ref="B36:F36"/>
     <mergeCell ref="A37:A40"/>
     <mergeCell ref="B37:F37"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="G5:G27"/>
-    <mergeCell ref="H5:H27"/>
-    <mergeCell ref="I5:I27"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B50:F50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3479,8 +3482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E4222C-B6F0-CA43-929A-A25489896A98}">
   <dimension ref="A1:G161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D80" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G99" sqref="G99:G141"/>
+    <sheetView tabSelected="1" topLeftCell="B134" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B157" sqref="B157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -3496,11 +3499,11 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="68" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A2" s="8" t="s">
@@ -3539,179 +3542,179 @@
       <c r="B5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="71" t="s">
+      <c r="C5" s="69" t="s">
         <v>155</v>
       </c>
-      <c r="D5" s="80">
+      <c r="D5" s="70">
         <v>1</v>
       </c>
       <c r="E5" s="17"/>
-      <c r="G5" s="76" t="s">
+      <c r="G5" s="74" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="79">
+      <c r="A6" s="71">
         <v>1.1000000000000001</v>
       </c>
       <c r="B6" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="80"/>
-      <c r="G6" s="77"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="70"/>
+      <c r="G6" s="75"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A7" s="79"/>
+      <c r="A7" s="71"/>
       <c r="B7" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="80"/>
-      <c r="G7" s="77"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="70"/>
+      <c r="G7" s="75"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A8" s="79"/>
+      <c r="A8" s="71"/>
       <c r="B8" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="71"/>
-      <c r="D8" s="80"/>
-      <c r="G8" s="77"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="70"/>
+      <c r="G8" s="75"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A9" s="79"/>
+      <c r="A9" s="71"/>
       <c r="B9" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="71"/>
-      <c r="D9" s="80"/>
-      <c r="G9" s="77"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="70"/>
+      <c r="G9" s="75"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A10" s="79">
+      <c r="A10" s="71">
         <v>1.2</v>
       </c>
       <c r="B10" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="80"/>
-      <c r="G10" s="77"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="70"/>
+      <c r="G10" s="75"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A11" s="79"/>
+      <c r="A11" s="71"/>
       <c r="B11" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="71"/>
-      <c r="D11" s="80"/>
-      <c r="G11" s="77"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="70"/>
+      <c r="G11" s="75"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A12" s="79"/>
+      <c r="A12" s="71"/>
       <c r="B12" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="71"/>
-      <c r="D12" s="80"/>
-      <c r="G12" s="77"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="70"/>
+      <c r="G12" s="75"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A13" s="79">
+      <c r="A13" s="71">
         <v>1.3</v>
       </c>
       <c r="B13" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="71"/>
-      <c r="D13" s="80"/>
-      <c r="G13" s="77"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="70"/>
+      <c r="G13" s="75"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A14" s="79"/>
+      <c r="A14" s="71"/>
       <c r="B14" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="71"/>
-      <c r="D14" s="80"/>
-      <c r="G14" s="77"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="70"/>
+      <c r="G14" s="75"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A15" s="79"/>
+      <c r="A15" s="71"/>
       <c r="B15" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="71"/>
-      <c r="D15" s="80"/>
-      <c r="G15" s="77"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="70"/>
+      <c r="G15" s="75"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A16" s="79"/>
+      <c r="A16" s="71"/>
       <c r="B16" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="71"/>
-      <c r="D16" s="80"/>
-      <c r="G16" s="77"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="70"/>
+      <c r="G16" s="75"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A17" s="79">
+      <c r="A17" s="71">
         <v>1.4</v>
       </c>
       <c r="B17" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="71"/>
-      <c r="D17" s="80"/>
-      <c r="G17" s="77"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="70"/>
+      <c r="G17" s="75"/>
     </row>
     <row r="18" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A18" s="79"/>
+      <c r="A18" s="71"/>
       <c r="B18" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="71"/>
-      <c r="D18" s="80"/>
-      <c r="G18" s="77"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="70"/>
+      <c r="G18" s="75"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A19" s="79"/>
+      <c r="A19" s="71"/>
       <c r="B19" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="71"/>
-      <c r="D19" s="80"/>
-      <c r="G19" s="77"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="70"/>
+      <c r="G19" s="75"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A20" s="79">
+      <c r="A20" s="71">
         <v>1.5</v>
       </c>
       <c r="B20" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="71"/>
-      <c r="D20" s="80"/>
-      <c r="G20" s="77"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="70"/>
+      <c r="G20" s="75"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A21" s="79"/>
+      <c r="A21" s="71"/>
       <c r="B21" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="71"/>
-      <c r="D21" s="80"/>
-      <c r="G21" s="77"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="70"/>
+      <c r="G21" s="75"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A22" s="79"/>
+      <c r="A22" s="71"/>
       <c r="B22" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="71"/>
-      <c r="D22" s="80"/>
-      <c r="G22" s="77"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="70"/>
+      <c r="G22" s="75"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A23" s="6">
@@ -3720,38 +3723,38 @@
       <c r="B23" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="71"/>
-      <c r="D23" s="80"/>
-      <c r="G23" s="77"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="70"/>
+      <c r="G23" s="75"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A24" s="79">
+      <c r="A24" s="71">
         <v>2.1</v>
       </c>
       <c r="B24" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="71"/>
-      <c r="D24" s="80"/>
-      <c r="G24" s="77"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="70"/>
+      <c r="G24" s="75"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A25" s="79"/>
+      <c r="A25" s="71"/>
       <c r="B25" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="71"/>
-      <c r="D25" s="80"/>
-      <c r="G25" s="77"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="70"/>
+      <c r="G25" s="75"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A26" s="79"/>
+      <c r="A26" s="71"/>
       <c r="B26" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="71"/>
-      <c r="D26" s="80"/>
-      <c r="G26" s="77"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="70"/>
+      <c r="G26" s="75"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A27" s="67">
@@ -3760,36 +3763,36 @@
       <c r="B27" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="71"/>
-      <c r="D27" s="80"/>
-      <c r="G27" s="77"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="70"/>
+      <c r="G27" s="75"/>
     </row>
     <row r="28" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A28" s="67"/>
       <c r="B28" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="71"/>
-      <c r="D28" s="80"/>
-      <c r="G28" s="77"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="70"/>
+      <c r="G28" s="75"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A29" s="67"/>
       <c r="B29" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="71"/>
-      <c r="D29" s="80"/>
-      <c r="G29" s="77"/>
+      <c r="C29" s="69"/>
+      <c r="D29" s="70"/>
+      <c r="G29" s="75"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A30" s="67"/>
       <c r="B30" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="71"/>
-      <c r="D30" s="80"/>
-      <c r="G30" s="77"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="70"/>
+      <c r="G30" s="75"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A31" s="67">
@@ -3798,27 +3801,27 @@
       <c r="B31" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="71"/>
-      <c r="D31" s="80"/>
-      <c r="G31" s="77"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="70"/>
+      <c r="G31" s="75"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A32" s="67"/>
       <c r="B32" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="71"/>
-      <c r="D32" s="80"/>
-      <c r="G32" s="77"/>
+      <c r="C32" s="69"/>
+      <c r="D32" s="70"/>
+      <c r="G32" s="75"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A33" s="67"/>
       <c r="B33" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="71"/>
-      <c r="D33" s="80"/>
-      <c r="G33" s="77"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="70"/>
+      <c r="G33" s="75"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A34" s="67">
@@ -3827,27 +3830,27 @@
       <c r="B34" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="71"/>
-      <c r="D34" s="80"/>
-      <c r="G34" s="77"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="70"/>
+      <c r="G34" s="75"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A35" s="67"/>
       <c r="B35" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="71"/>
-      <c r="D35" s="80"/>
-      <c r="G35" s="77"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="70"/>
+      <c r="G35" s="75"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A36" s="67"/>
       <c r="B36" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="71"/>
-      <c r="D36" s="80"/>
-      <c r="G36" s="77"/>
+      <c r="C36" s="69"/>
+      <c r="D36" s="70"/>
+      <c r="G36" s="75"/>
     </row>
     <row r="37" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A37" s="6">
@@ -3856,9 +3859,9 @@
       <c r="B37" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="71"/>
-      <c r="D37" s="80"/>
-      <c r="G37" s="77"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="70"/>
+      <c r="G37" s="75"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A38" s="67">
@@ -3867,27 +3870,27 @@
       <c r="B38" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="71"/>
-      <c r="D38" s="80"/>
-      <c r="G38" s="77"/>
+      <c r="C38" s="69"/>
+      <c r="D38" s="70"/>
+      <c r="G38" s="75"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A39" s="67"/>
       <c r="B39" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="71"/>
-      <c r="D39" s="80"/>
-      <c r="G39" s="77"/>
+      <c r="C39" s="69"/>
+      <c r="D39" s="70"/>
+      <c r="G39" s="75"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A40" s="67"/>
       <c r="B40" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="71"/>
-      <c r="D40" s="80"/>
-      <c r="G40" s="77"/>
+      <c r="C40" s="69"/>
+      <c r="D40" s="70"/>
+      <c r="G40" s="75"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A41" s="67">
@@ -3896,27 +3899,27 @@
       <c r="B41" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="71"/>
-      <c r="D41" s="80"/>
-      <c r="G41" s="77"/>
+      <c r="C41" s="69"/>
+      <c r="D41" s="70"/>
+      <c r="G41" s="75"/>
     </row>
     <row r="42" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A42" s="67"/>
       <c r="B42" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="71"/>
-      <c r="D42" s="80"/>
-      <c r="G42" s="77"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="70"/>
+      <c r="G42" s="75"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A43" s="67"/>
       <c r="B43" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="71"/>
-      <c r="D43" s="80"/>
-      <c r="G43" s="77"/>
+      <c r="C43" s="69"/>
+      <c r="D43" s="70"/>
+      <c r="G43" s="75"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A44" s="67">
@@ -3925,27 +3928,27 @@
       <c r="B44" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="71"/>
-      <c r="D44" s="80"/>
-      <c r="G44" s="77"/>
+      <c r="C44" s="69"/>
+      <c r="D44" s="70"/>
+      <c r="G44" s="75"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A45" s="67"/>
       <c r="B45" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="71"/>
-      <c r="D45" s="80"/>
-      <c r="G45" s="77"/>
+      <c r="C45" s="69"/>
+      <c r="D45" s="70"/>
+      <c r="G45" s="75"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A46" s="67"/>
       <c r="B46" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="71"/>
-      <c r="D46" s="80"/>
-      <c r="G46" s="77"/>
+      <c r="C46" s="69"/>
+      <c r="D46" s="70"/>
+      <c r="G46" s="75"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A47" s="67">
@@ -3954,27 +3957,27 @@
       <c r="B47" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="71"/>
-      <c r="D47" s="80"/>
-      <c r="G47" s="77"/>
+      <c r="C47" s="69"/>
+      <c r="D47" s="70"/>
+      <c r="G47" s="75"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A48" s="67"/>
       <c r="B48" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="71"/>
-      <c r="D48" s="80"/>
-      <c r="G48" s="77"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="70"/>
+      <c r="G48" s="75"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A49" s="67"/>
       <c r="B49" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="C49" s="71"/>
-      <c r="D49" s="80"/>
-      <c r="G49" s="77"/>
+      <c r="C49" s="69"/>
+      <c r="D49" s="70"/>
+      <c r="G49" s="75"/>
     </row>
     <row r="50" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A50" s="6">
@@ -3983,10 +3986,10 @@
       <c r="B50" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="C50" s="71" t="s">
+      <c r="C50" s="69" t="s">
         <v>157</v>
       </c>
-      <c r="D50" s="80">
+      <c r="D50" s="70">
         <v>1</v>
       </c>
       <c r="E50" s="17"/>
@@ -4001,8 +4004,8 @@
       <c r="B51" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="71"/>
-      <c r="D51" s="80"/>
+      <c r="C51" s="69"/>
+      <c r="D51" s="70"/>
       <c r="G51" s="72"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.6">
@@ -4010,8 +4013,8 @@
       <c r="B52" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="C52" s="71"/>
-      <c r="D52" s="80"/>
+      <c r="C52" s="69"/>
+      <c r="D52" s="70"/>
       <c r="G52" s="72"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.6">
@@ -4019,8 +4022,8 @@
       <c r="B53" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="C53" s="71"/>
-      <c r="D53" s="80"/>
+      <c r="C53" s="69"/>
+      <c r="D53" s="70"/>
       <c r="G53" s="72"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.6">
@@ -4028,8 +4031,8 @@
       <c r="B54" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C54" s="71"/>
-      <c r="D54" s="80"/>
+      <c r="C54" s="69"/>
+      <c r="D54" s="70"/>
       <c r="G54" s="72"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.6">
@@ -4039,8 +4042,8 @@
       <c r="B55" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C55" s="71"/>
-      <c r="D55" s="80"/>
+      <c r="C55" s="69"/>
+      <c r="D55" s="70"/>
       <c r="G55" s="72"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.6">
@@ -4048,8 +4051,8 @@
       <c r="B56" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="C56" s="71"/>
-      <c r="D56" s="80"/>
+      <c r="C56" s="69"/>
+      <c r="D56" s="70"/>
       <c r="G56" s="72"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.6">
@@ -4057,8 +4060,8 @@
       <c r="B57" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="C57" s="71"/>
-      <c r="D57" s="80"/>
+      <c r="C57" s="69"/>
+      <c r="D57" s="70"/>
       <c r="G57" s="72"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.6">
@@ -4068,8 +4071,8 @@
       <c r="B58" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C58" s="71"/>
-      <c r="D58" s="80"/>
+      <c r="C58" s="69"/>
+      <c r="D58" s="70"/>
       <c r="G58" s="72"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.6">
@@ -4077,8 +4080,8 @@
       <c r="B59" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C59" s="71"/>
-      <c r="D59" s="80"/>
+      <c r="C59" s="69"/>
+      <c r="D59" s="70"/>
       <c r="G59" s="72"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.6">
@@ -4086,8 +4089,8 @@
       <c r="B60" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="C60" s="71"/>
-      <c r="D60" s="80"/>
+      <c r="C60" s="69"/>
+      <c r="D60" s="70"/>
       <c r="G60" s="72"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.6">
@@ -4097,8 +4100,8 @@
       <c r="B61" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="C61" s="71"/>
-      <c r="D61" s="80"/>
+      <c r="C61" s="69"/>
+      <c r="D61" s="70"/>
       <c r="G61" s="72"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.6">
@@ -4106,8 +4109,8 @@
       <c r="B62" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="C62" s="71"/>
-      <c r="D62" s="80"/>
+      <c r="C62" s="69"/>
+      <c r="D62" s="70"/>
       <c r="G62" s="72"/>
     </row>
     <row r="63" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
@@ -4115,8 +4118,8 @@
       <c r="B63" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="C63" s="71"/>
-      <c r="D63" s="80"/>
+      <c r="C63" s="69"/>
+      <c r="D63" s="70"/>
       <c r="G63" s="72"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.6">
@@ -4124,8 +4127,8 @@
       <c r="B64" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="C64" s="71"/>
-      <c r="D64" s="80"/>
+      <c r="C64" s="69"/>
+      <c r="D64" s="70"/>
       <c r="G64" s="72"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.6">
@@ -4135,8 +4138,8 @@
       <c r="B65" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="C65" s="71"/>
-      <c r="D65" s="80"/>
+      <c r="C65" s="69"/>
+      <c r="D65" s="70"/>
       <c r="G65" s="72"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.6">
@@ -4146,8 +4149,8 @@
       <c r="B66" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="C66" s="71"/>
-      <c r="D66" s="80"/>
+      <c r="C66" s="69"/>
+      <c r="D66" s="70"/>
       <c r="G66" s="72"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.6">
@@ -4155,8 +4158,8 @@
       <c r="B67" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="C67" s="71"/>
-      <c r="D67" s="80"/>
+      <c r="C67" s="69"/>
+      <c r="D67" s="70"/>
       <c r="G67" s="72"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.6">
@@ -4164,8 +4167,8 @@
       <c r="B68" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C68" s="71"/>
-      <c r="D68" s="80"/>
+      <c r="C68" s="69"/>
+      <c r="D68" s="70"/>
       <c r="G68" s="72"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.6">
@@ -4175,8 +4178,8 @@
       <c r="B69" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C69" s="71"/>
-      <c r="D69" s="80"/>
+      <c r="C69" s="69"/>
+      <c r="D69" s="70"/>
       <c r="G69" s="72"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.6">
@@ -4184,8 +4187,8 @@
       <c r="B70" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C70" s="71"/>
-      <c r="D70" s="80"/>
+      <c r="C70" s="69"/>
+      <c r="D70" s="70"/>
       <c r="G70" s="72"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.6">
@@ -4193,8 +4196,8 @@
       <c r="B71" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="C71" s="71"/>
-      <c r="D71" s="80"/>
+      <c r="C71" s="69"/>
+      <c r="D71" s="70"/>
       <c r="G71" s="72"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.6">
@@ -4204,8 +4207,8 @@
       <c r="B72" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="C72" s="71"/>
-      <c r="D72" s="80"/>
+      <c r="C72" s="69"/>
+      <c r="D72" s="70"/>
       <c r="G72" s="72"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.6">
@@ -4213,8 +4216,8 @@
       <c r="B73" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="C73" s="71"/>
-      <c r="D73" s="80"/>
+      <c r="C73" s="69"/>
+      <c r="D73" s="70"/>
       <c r="G73" s="72"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.6">
@@ -4222,8 +4225,8 @@
       <c r="B74" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="C74" s="71"/>
-      <c r="D74" s="80"/>
+      <c r="C74" s="69"/>
+      <c r="D74" s="70"/>
       <c r="G74" s="72"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.6">
@@ -4233,8 +4236,8 @@
       <c r="B75" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="C75" s="71"/>
-      <c r="D75" s="80"/>
+      <c r="C75" s="69"/>
+      <c r="D75" s="70"/>
       <c r="G75" s="72"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.6">
@@ -4242,8 +4245,8 @@
       <c r="B76" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="C76" s="71"/>
-      <c r="D76" s="80"/>
+      <c r="C76" s="69"/>
+      <c r="D76" s="70"/>
       <c r="G76" s="72"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.6">
@@ -4251,8 +4254,8 @@
       <c r="B77" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="C77" s="71"/>
-      <c r="D77" s="80"/>
+      <c r="C77" s="69"/>
+      <c r="D77" s="70"/>
       <c r="G77" s="72"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.6">
@@ -4262,55 +4265,55 @@
       <c r="B78" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C78" s="71"/>
-      <c r="D78" s="80"/>
+      <c r="C78" s="69"/>
+      <c r="D78" s="70"/>
       <c r="G78" s="72"/>
     </row>
     <row r="79" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A79" s="79">
+      <c r="A79" s="71">
         <v>6.1</v>
       </c>
       <c r="B79" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="C79" s="71"/>
-      <c r="D79" s="80"/>
+      <c r="C79" s="69"/>
+      <c r="D79" s="70"/>
       <c r="G79" s="72"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A80" s="79"/>
+      <c r="A80" s="71"/>
       <c r="B80" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="C80" s="71"/>
-      <c r="D80" s="80"/>
+      <c r="C80" s="69"/>
+      <c r="D80" s="70"/>
       <c r="G80" s="72"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A81" s="79"/>
+      <c r="A81" s="71"/>
       <c r="B81" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="C81" s="71"/>
-      <c r="D81" s="80"/>
+      <c r="C81" s="69"/>
+      <c r="D81" s="70"/>
       <c r="G81" s="72"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A82" s="79"/>
+      <c r="A82" s="71"/>
       <c r="B82" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="C82" s="71"/>
-      <c r="D82" s="80"/>
+      <c r="C82" s="69"/>
+      <c r="D82" s="70"/>
       <c r="G82" s="72"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A83" s="79"/>
+      <c r="A83" s="71"/>
       <c r="B83" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="C83" s="71"/>
-      <c r="D83" s="80"/>
+      <c r="C83" s="69"/>
+      <c r="D83" s="70"/>
       <c r="G83" s="72"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.6">
@@ -4320,8 +4323,8 @@
       <c r="B84" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="C84" s="71"/>
-      <c r="D84" s="80"/>
+      <c r="C84" s="69"/>
+      <c r="D84" s="70"/>
       <c r="G84" s="72"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.6">
@@ -4329,8 +4332,8 @@
       <c r="B85" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C85" s="71"/>
-      <c r="D85" s="80"/>
+      <c r="C85" s="69"/>
+      <c r="D85" s="70"/>
       <c r="G85" s="72"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.6">
@@ -4338,8 +4341,8 @@
       <c r="B86" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="C86" s="71"/>
-      <c r="D86" s="80"/>
+      <c r="C86" s="69"/>
+      <c r="D86" s="70"/>
       <c r="G86" s="72"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.6">
@@ -4347,8 +4350,8 @@
       <c r="B87" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="C87" s="71"/>
-      <c r="D87" s="80"/>
+      <c r="C87" s="69"/>
+      <c r="D87" s="70"/>
       <c r="G87" s="72"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.6">
@@ -4356,8 +4359,8 @@
       <c r="B88" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="C88" s="71"/>
-      <c r="D88" s="80"/>
+      <c r="C88" s="69"/>
+      <c r="D88" s="70"/>
       <c r="G88" s="72"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.6">
@@ -4367,8 +4370,8 @@
       <c r="B89" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="C89" s="71"/>
-      <c r="D89" s="80"/>
+      <c r="C89" s="69"/>
+      <c r="D89" s="70"/>
       <c r="G89" s="72"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.6">
@@ -4376,8 +4379,8 @@
       <c r="B90" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="C90" s="71"/>
-      <c r="D90" s="80"/>
+      <c r="C90" s="69"/>
+      <c r="D90" s="70"/>
       <c r="G90" s="72"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.6">
@@ -4385,8 +4388,8 @@
       <c r="B91" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="C91" s="71"/>
-      <c r="D91" s="80"/>
+      <c r="C91" s="69"/>
+      <c r="D91" s="70"/>
       <c r="G91" s="72"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.6">
@@ -4396,8 +4399,8 @@
       <c r="B92" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="C92" s="71"/>
-      <c r="D92" s="80"/>
+      <c r="C92" s="69"/>
+      <c r="D92" s="70"/>
       <c r="G92" s="72"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.6">
@@ -4405,8 +4408,8 @@
       <c r="B93" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="C93" s="71"/>
-      <c r="D93" s="80"/>
+      <c r="C93" s="69"/>
+      <c r="D93" s="70"/>
       <c r="G93" s="72"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.6">
@@ -4414,8 +4417,8 @@
       <c r="B94" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="C94" s="71"/>
-      <c r="D94" s="80"/>
+      <c r="C94" s="69"/>
+      <c r="D94" s="70"/>
       <c r="G94" s="72"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.6">
@@ -4425,8 +4428,8 @@
       <c r="B95" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="C95" s="71"/>
-      <c r="D95" s="80"/>
+      <c r="C95" s="69"/>
+      <c r="D95" s="70"/>
       <c r="G95" s="72"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.6">
@@ -4434,8 +4437,8 @@
       <c r="B96" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="C96" s="71"/>
-      <c r="D96" s="80"/>
+      <c r="C96" s="69"/>
+      <c r="D96" s="70"/>
       <c r="G96" s="72"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.6">
@@ -4443,8 +4446,8 @@
       <c r="B97" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="C97" s="71"/>
-      <c r="D97" s="80"/>
+      <c r="C97" s="69"/>
+      <c r="D97" s="70"/>
       <c r="G97" s="72"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.6">
@@ -4452,8 +4455,8 @@
       <c r="B98" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="C98" s="71"/>
-      <c r="D98" s="80"/>
+      <c r="C98" s="69"/>
+      <c r="D98" s="70"/>
       <c r="G98" s="72"/>
     </row>
     <row r="99" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
@@ -4463,132 +4466,132 @@
       <c r="B99" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C99" s="74" t="s">
+      <c r="C99" s="73" t="s">
         <v>159</v>
       </c>
-      <c r="D99" s="68">
+      <c r="D99" s="78">
         <v>1</v>
       </c>
       <c r="E99" s="17"/>
-      <c r="G99" s="70" t="s">
+      <c r="G99" s="76" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A100" s="78">
+      <c r="A100" s="77">
         <v>7.1</v>
       </c>
       <c r="B100" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="C100" s="74"/>
-      <c r="D100" s="68"/>
-      <c r="G100" s="70"/>
+      <c r="C100" s="73"/>
+      <c r="D100" s="78"/>
+      <c r="G100" s="76"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A101" s="78"/>
+      <c r="A101" s="77"/>
       <c r="B101" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="C101" s="74"/>
-      <c r="D101" s="68"/>
-      <c r="G101" s="70"/>
+      <c r="C101" s="73"/>
+      <c r="D101" s="78"/>
+      <c r="G101" s="76"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A102" s="78"/>
+      <c r="A102" s="77"/>
       <c r="B102" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="C102" s="74"/>
-      <c r="D102" s="68"/>
-      <c r="G102" s="70"/>
+      <c r="C102" s="73"/>
+      <c r="D102" s="78"/>
+      <c r="G102" s="76"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A103" s="78">
+      <c r="A103" s="77">
         <v>7.2</v>
       </c>
       <c r="B103" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="C103" s="74"/>
-      <c r="D103" s="68"/>
-      <c r="G103" s="70"/>
+      <c r="C103" s="73"/>
+      <c r="D103" s="78"/>
+      <c r="G103" s="76"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A104" s="78"/>
+      <c r="A104" s="77"/>
       <c r="B104" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="C104" s="74"/>
-      <c r="D104" s="68"/>
-      <c r="G104" s="70"/>
+      <c r="C104" s="73"/>
+      <c r="D104" s="78"/>
+      <c r="G104" s="76"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A105" s="78"/>
+      <c r="A105" s="77"/>
       <c r="B105" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="C105" s="74"/>
-      <c r="D105" s="68"/>
-      <c r="G105" s="70"/>
+      <c r="C105" s="73"/>
+      <c r="D105" s="78"/>
+      <c r="G105" s="76"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A106" s="78">
+      <c r="A106" s="77">
         <v>7.3</v>
       </c>
       <c r="B106" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="C106" s="74"/>
-      <c r="D106" s="68"/>
-      <c r="G106" s="70"/>
+      <c r="C106" s="73"/>
+      <c r="D106" s="78"/>
+      <c r="G106" s="76"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A107" s="78"/>
+      <c r="A107" s="77"/>
       <c r="B107" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="C107" s="74"/>
-      <c r="D107" s="68"/>
-      <c r="G107" s="70"/>
+      <c r="C107" s="73"/>
+      <c r="D107" s="78"/>
+      <c r="G107" s="76"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A108" s="78"/>
+      <c r="A108" s="77"/>
       <c r="B108" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C108" s="74"/>
-      <c r="D108" s="68"/>
-      <c r="G108" s="70"/>
+      <c r="C108" s="73"/>
+      <c r="D108" s="78"/>
+      <c r="G108" s="76"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A109" s="78">
+      <c r="A109" s="77">
         <v>7.4</v>
       </c>
       <c r="B109" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="C109" s="74"/>
-      <c r="D109" s="68"/>
-      <c r="G109" s="70"/>
+      <c r="C109" s="73"/>
+      <c r="D109" s="78"/>
+      <c r="G109" s="76"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A110" s="78"/>
+      <c r="A110" s="77"/>
       <c r="B110" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="C110" s="74"/>
-      <c r="D110" s="68"/>
-      <c r="G110" s="70"/>
+      <c r="C110" s="73"/>
+      <c r="D110" s="78"/>
+      <c r="G110" s="76"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A111" s="78"/>
+      <c r="A111" s="77"/>
       <c r="B111" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="C111" s="74"/>
-      <c r="D111" s="68"/>
-      <c r="G111" s="70"/>
+      <c r="C111" s="73"/>
+      <c r="D111" s="78"/>
+      <c r="G111" s="76"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A112" s="5">
@@ -4597,9 +4600,9 @@
       <c r="B112" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C112" s="74"/>
-      <c r="D112" s="68"/>
-      <c r="G112" s="70"/>
+      <c r="C112" s="73"/>
+      <c r="D112" s="78"/>
+      <c r="G112" s="76"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A113" s="33">
@@ -4608,101 +4611,101 @@
       <c r="B113" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="C113" s="74"/>
-      <c r="D113" s="68"/>
-      <c r="G113" s="70"/>
+      <c r="C113" s="73"/>
+      <c r="D113" s="78"/>
+      <c r="G113" s="76"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A114" s="78">
+      <c r="A114" s="77">
         <v>8.1</v>
       </c>
       <c r="B114" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="C114" s="74"/>
-      <c r="D114" s="68"/>
-      <c r="G114" s="70"/>
+      <c r="C114" s="73"/>
+      <c r="D114" s="78"/>
+      <c r="G114" s="76"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A115" s="78"/>
+      <c r="A115" s="77"/>
       <c r="B115" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="C115" s="74"/>
-      <c r="D115" s="68"/>
-      <c r="G115" s="70"/>
+      <c r="C115" s="73"/>
+      <c r="D115" s="78"/>
+      <c r="G115" s="76"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A116" s="78"/>
+      <c r="A116" s="77"/>
       <c r="B116" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="C116" s="74"/>
-      <c r="D116" s="68"/>
-      <c r="G116" s="70"/>
+      <c r="C116" s="73"/>
+      <c r="D116" s="78"/>
+      <c r="G116" s="76"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A117" s="78"/>
+      <c r="A117" s="77"/>
       <c r="B117" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="C117" s="74"/>
-      <c r="D117" s="68"/>
-      <c r="G117" s="70"/>
+      <c r="C117" s="73"/>
+      <c r="D117" s="78"/>
+      <c r="G117" s="76"/>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A118" s="78"/>
+      <c r="A118" s="77"/>
       <c r="B118" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="C118" s="74"/>
-      <c r="D118" s="68"/>
-      <c r="G118" s="70"/>
+      <c r="C118" s="73"/>
+      <c r="D118" s="78"/>
+      <c r="G118" s="76"/>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A119" s="78"/>
+      <c r="A119" s="77"/>
       <c r="B119" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="C119" s="74"/>
-      <c r="D119" s="68"/>
-      <c r="G119" s="70"/>
+      <c r="C119" s="73"/>
+      <c r="D119" s="78"/>
+      <c r="G119" s="76"/>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A120" s="78"/>
+      <c r="A120" s="77"/>
       <c r="B120" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="C120" s="74"/>
-      <c r="D120" s="68"/>
-      <c r="G120" s="70"/>
+      <c r="C120" s="73"/>
+      <c r="D120" s="78"/>
+      <c r="G120" s="76"/>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A121" s="67"/>
       <c r="B121" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="C121" s="74"/>
-      <c r="D121" s="68"/>
-      <c r="G121" s="70"/>
+      <c r="C121" s="73"/>
+      <c r="D121" s="78"/>
+      <c r="G121" s="76"/>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A122" s="67"/>
       <c r="B122" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="C122" s="74"/>
-      <c r="D122" s="68"/>
-      <c r="G122" s="70"/>
+      <c r="C122" s="73"/>
+      <c r="D122" s="78"/>
+      <c r="G122" s="76"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A123" s="67"/>
       <c r="B123" s="36" t="s">
         <v>152</v>
       </c>
-      <c r="C123" s="74"/>
-      <c r="D123" s="68"/>
-      <c r="G123" s="70"/>
+      <c r="C123" s="73"/>
+      <c r="D123" s="78"/>
+      <c r="G123" s="76"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A124" s="32">
@@ -4711,61 +4714,61 @@
       <c r="B124" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="C124" s="74" t="s">
+      <c r="C124" s="73" t="s">
         <v>168</v>
       </c>
-      <c r="D124" s="68">
+      <c r="D124" s="78">
         <v>0.75</v>
       </c>
       <c r="E124" s="17"/>
-      <c r="G124" s="70"/>
+      <c r="G124" s="76"/>
     </row>
     <row r="125" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A125" s="69">
+      <c r="A125" s="81">
         <v>9.1</v>
       </c>
       <c r="B125" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="C125" s="74"/>
-      <c r="D125" s="68"/>
-      <c r="G125" s="70"/>
+      <c r="C125" s="73"/>
+      <c r="D125" s="78"/>
+      <c r="G125" s="76"/>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A126" s="69"/>
+      <c r="A126" s="81"/>
       <c r="B126" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="C126" s="74"/>
-      <c r="D126" s="68"/>
-      <c r="G126" s="70"/>
+      <c r="C126" s="73"/>
+      <c r="D126" s="78"/>
+      <c r="G126" s="76"/>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A127" s="69"/>
+      <c r="A127" s="81"/>
       <c r="B127" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="C127" s="74"/>
-      <c r="D127" s="68"/>
-      <c r="G127" s="70"/>
+      <c r="C127" s="73"/>
+      <c r="D127" s="78"/>
+      <c r="G127" s="76"/>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A128" s="69"/>
+      <c r="A128" s="81"/>
       <c r="B128" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="C128" s="74"/>
-      <c r="D128" s="68"/>
-      <c r="G128" s="70"/>
+      <c r="C128" s="73"/>
+      <c r="D128" s="78"/>
+      <c r="G128" s="76"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A129" s="69"/>
+      <c r="A129" s="81"/>
       <c r="B129" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="C129" s="74"/>
-      <c r="D129" s="68"/>
-      <c r="G129" s="70"/>
+      <c r="C129" s="73"/>
+      <c r="D129" s="78"/>
+      <c r="G129" s="76"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A130" s="67">
@@ -4774,36 +4777,36 @@
       <c r="B130" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="C130" s="74"/>
-      <c r="D130" s="68"/>
-      <c r="G130" s="70"/>
+      <c r="C130" s="73"/>
+      <c r="D130" s="78"/>
+      <c r="G130" s="76"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A131" s="67"/>
       <c r="B131" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="C131" s="74"/>
-      <c r="D131" s="68"/>
-      <c r="G131" s="70"/>
+      <c r="C131" s="73"/>
+      <c r="D131" s="78"/>
+      <c r="G131" s="76"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A132" s="67"/>
       <c r="B132" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="C132" s="74"/>
-      <c r="D132" s="68"/>
-      <c r="G132" s="70"/>
+      <c r="C132" s="73"/>
+      <c r="D132" s="78"/>
+      <c r="G132" s="76"/>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A133" s="67"/>
       <c r="B133" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="C133" s="74"/>
-      <c r="D133" s="68"/>
-      <c r="G133" s="70"/>
+      <c r="C133" s="73"/>
+      <c r="D133" s="78"/>
+      <c r="G133" s="76"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A134" s="67">
@@ -4812,36 +4815,36 @@
       <c r="B134" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="C134" s="74"/>
-      <c r="D134" s="68"/>
-      <c r="G134" s="70"/>
+      <c r="C134" s="73"/>
+      <c r="D134" s="78"/>
+      <c r="G134" s="76"/>
     </row>
     <row r="135" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A135" s="67"/>
       <c r="B135" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="C135" s="74"/>
-      <c r="D135" s="68"/>
-      <c r="G135" s="70"/>
+      <c r="C135" s="73"/>
+      <c r="D135" s="78"/>
+      <c r="G135" s="76"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A136" s="67"/>
       <c r="B136" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C136" s="74"/>
-      <c r="D136" s="68"/>
-      <c r="G136" s="70"/>
+      <c r="C136" s="73"/>
+      <c r="D136" s="78"/>
+      <c r="G136" s="76"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A137" s="67"/>
       <c r="B137" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="C137" s="74"/>
-      <c r="D137" s="68"/>
-      <c r="G137" s="70"/>
+      <c r="C137" s="73"/>
+      <c r="D137" s="78"/>
+      <c r="G137" s="76"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A138" s="67">
@@ -4850,36 +4853,36 @@
       <c r="B138" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="C138" s="74"/>
-      <c r="D138" s="68"/>
-      <c r="G138" s="70"/>
+      <c r="C138" s="73"/>
+      <c r="D138" s="78"/>
+      <c r="G138" s="76"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A139" s="67"/>
       <c r="B139" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="C139" s="74"/>
-      <c r="D139" s="68"/>
-      <c r="G139" s="70"/>
+      <c r="C139" s="73"/>
+      <c r="D139" s="78"/>
+      <c r="G139" s="76"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A140" s="67"/>
       <c r="B140" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="C140" s="74"/>
-      <c r="D140" s="68"/>
-      <c r="G140" s="70"/>
+      <c r="C140" s="73"/>
+      <c r="D140" s="78"/>
+      <c r="G140" s="76"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A141" s="67"/>
       <c r="B141" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="C141" s="74"/>
-      <c r="D141" s="68"/>
-      <c r="G141" s="70"/>
+      <c r="C141" s="73"/>
+      <c r="D141" s="78"/>
+      <c r="G141" s="76"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A142" s="6">
@@ -4888,14 +4891,14 @@
       <c r="B142" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="C142" s="71" t="s">
+      <c r="C142" s="69" t="s">
         <v>169</v>
       </c>
-      <c r="D142" s="68">
+      <c r="D142" s="78">
         <v>1.75</v>
       </c>
       <c r="E142" s="17"/>
-      <c r="G142" s="70"/>
+      <c r="G142" s="76"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A143" s="5">
@@ -4904,9 +4907,9 @@
       <c r="B143" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="C143" s="71"/>
-      <c r="D143" s="68"/>
-      <c r="G143" s="70"/>
+      <c r="C143" s="69"/>
+      <c r="D143" s="78"/>
+      <c r="G143" s="76"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A144" s="6">
@@ -4915,10 +4918,10 @@
       <c r="B144" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="C144" s="74" t="s">
+      <c r="C144" s="73" t="s">
         <v>170</v>
       </c>
-      <c r="D144" s="68">
+      <c r="D144" s="78">
         <v>0.5</v>
       </c>
       <c r="E144" s="17"/>
@@ -4931,8 +4934,8 @@
       <c r="B145" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C145" s="75"/>
-      <c r="D145" s="68"/>
+      <c r="C145" s="80"/>
+      <c r="D145" s="78"/>
       <c r="G145" s="72"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.6">
@@ -4940,8 +4943,8 @@
       <c r="B146" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C146" s="75"/>
-      <c r="D146" s="68"/>
+      <c r="C146" s="80"/>
+      <c r="D146" s="78"/>
       <c r="G146" s="72"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.6">
@@ -4949,8 +4952,8 @@
       <c r="B147" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C147" s="75"/>
-      <c r="D147" s="68"/>
+      <c r="C147" s="80"/>
+      <c r="D147" s="78"/>
       <c r="G147" s="72"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.6">
@@ -4960,8 +4963,8 @@
       <c r="B148" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C148" s="75"/>
-      <c r="D148" s="68"/>
+      <c r="C148" s="80"/>
+      <c r="D148" s="78"/>
       <c r="G148" s="72"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.6">
@@ -4969,8 +4972,8 @@
       <c r="B149" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C149" s="75"/>
-      <c r="D149" s="68"/>
+      <c r="C149" s="80"/>
+      <c r="D149" s="78"/>
       <c r="G149" s="72"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.6">
@@ -4978,117 +4981,159 @@
       <c r="B150" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C150" s="75"/>
-      <c r="D150" s="68"/>
+      <c r="C150" s="80"/>
+      <c r="D150" s="78"/>
       <c r="G150" s="72"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A151" s="73">
+      <c r="A151" s="79">
         <v>11.3</v>
       </c>
       <c r="B151" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="C151" s="75"/>
-      <c r="D151" s="68"/>
+      <c r="C151" s="80"/>
+      <c r="D151" s="78"/>
       <c r="G151" s="72"/>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A152" s="73"/>
+      <c r="A152" s="79"/>
       <c r="B152" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C152" s="75"/>
-      <c r="D152" s="68"/>
+      <c r="C152" s="80"/>
+      <c r="D152" s="78"/>
       <c r="G152" s="72"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A153" s="73"/>
+      <c r="A153" s="79"/>
       <c r="B153" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C153" s="75"/>
-      <c r="D153" s="68"/>
+      <c r="C153" s="80"/>
+      <c r="D153" s="78"/>
       <c r="G153" s="72"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A154" s="73"/>
+      <c r="A154" s="79"/>
       <c r="B154" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C154" s="75"/>
-      <c r="D154" s="68"/>
+      <c r="C154" s="80"/>
+      <c r="D154" s="78"/>
       <c r="G154" s="72"/>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A155" s="73">
+      <c r="A155" s="79">
         <v>11.4</v>
       </c>
       <c r="B155" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="C155" s="75"/>
-      <c r="D155" s="68"/>
+      <c r="C155" s="80"/>
+      <c r="D155" s="78"/>
       <c r="G155" s="72"/>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A156" s="73"/>
+      <c r="A156" s="79"/>
       <c r="B156" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="C156" s="75"/>
-      <c r="D156" s="68"/>
+      <c r="C156" s="80"/>
+      <c r="D156" s="78"/>
       <c r="G156" s="72"/>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A157" s="73"/>
+      <c r="A157" s="79"/>
       <c r="B157" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="C157" s="75"/>
-      <c r="D157" s="68"/>
+      <c r="C157" s="80"/>
+      <c r="D157" s="78"/>
       <c r="G157" s="72"/>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A158" s="73">
+      <c r="A158" s="79">
         <v>11.5</v>
       </c>
       <c r="B158" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="C158" s="75"/>
-      <c r="D158" s="68"/>
+      <c r="C158" s="80"/>
+      <c r="D158" s="78"/>
       <c r="G158" s="72"/>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A159" s="73"/>
+      <c r="A159" s="79"/>
       <c r="B159" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="C159" s="75"/>
-      <c r="D159" s="68"/>
+      <c r="C159" s="80"/>
+      <c r="D159" s="78"/>
       <c r="G159" s="72"/>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A160" s="73"/>
-      <c r="B160" s="30" t="s">
+      <c r="A160" s="79"/>
+      <c r="B160" s="82" t="s">
         <v>141</v>
       </c>
-      <c r="C160" s="75"/>
-      <c r="D160" s="68"/>
+      <c r="C160" s="80"/>
+      <c r="D160" s="78"/>
       <c r="G160" s="72"/>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A161" s="73"/>
+      <c r="A161" s="79"/>
       <c r="B161" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="C161" s="75"/>
-      <c r="D161" s="68"/>
+      <c r="C161" s="80"/>
+      <c r="D161" s="78"/>
       <c r="G161" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="A130:A133"/>
+    <mergeCell ref="A134:A137"/>
+    <mergeCell ref="A138:A141"/>
+    <mergeCell ref="D124:D141"/>
+    <mergeCell ref="A125:A129"/>
+    <mergeCell ref="G142:G143"/>
+    <mergeCell ref="C142:C143"/>
+    <mergeCell ref="D142:D143"/>
+    <mergeCell ref="A145:A147"/>
+    <mergeCell ref="G144:G161"/>
+    <mergeCell ref="D144:D161"/>
+    <mergeCell ref="A148:A150"/>
+    <mergeCell ref="A151:A154"/>
+    <mergeCell ref="A155:A157"/>
+    <mergeCell ref="A158:A161"/>
+    <mergeCell ref="C144:C161"/>
+    <mergeCell ref="C99:C123"/>
+    <mergeCell ref="G5:G49"/>
+    <mergeCell ref="G99:G141"/>
+    <mergeCell ref="A100:A102"/>
+    <mergeCell ref="A103:A105"/>
+    <mergeCell ref="A106:A108"/>
+    <mergeCell ref="A109:A111"/>
+    <mergeCell ref="A114:A123"/>
+    <mergeCell ref="C124:C141"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A79:A83"/>
+    <mergeCell ref="A84:A88"/>
+    <mergeCell ref="A89:A91"/>
+    <mergeCell ref="A92:A94"/>
+    <mergeCell ref="D99:D123"/>
+    <mergeCell ref="C50:C98"/>
+    <mergeCell ref="D50:D98"/>
+    <mergeCell ref="G50:G98"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="A95:A98"/>
     <mergeCell ref="A44:A46"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="C5:C49"/>
@@ -5105,48 +5150,6 @@
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A38:A40"/>
     <mergeCell ref="A41:A43"/>
-    <mergeCell ref="C50:C98"/>
-    <mergeCell ref="D50:D98"/>
-    <mergeCell ref="G50:G98"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="C99:C123"/>
-    <mergeCell ref="G5:G49"/>
-    <mergeCell ref="G99:G141"/>
-    <mergeCell ref="A100:A102"/>
-    <mergeCell ref="A103:A105"/>
-    <mergeCell ref="A106:A108"/>
-    <mergeCell ref="A109:A111"/>
-    <mergeCell ref="A114:A123"/>
-    <mergeCell ref="C124:C141"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A79:A83"/>
-    <mergeCell ref="A84:A88"/>
-    <mergeCell ref="A89:A91"/>
-    <mergeCell ref="A92:A94"/>
-    <mergeCell ref="D99:D123"/>
-    <mergeCell ref="G142:G143"/>
-    <mergeCell ref="C142:C143"/>
-    <mergeCell ref="D142:D143"/>
-    <mergeCell ref="A145:A147"/>
-    <mergeCell ref="G144:G161"/>
-    <mergeCell ref="D144:D161"/>
-    <mergeCell ref="A148:A150"/>
-    <mergeCell ref="A151:A154"/>
-    <mergeCell ref="A155:A157"/>
-    <mergeCell ref="A158:A161"/>
-    <mergeCell ref="C144:C161"/>
-    <mergeCell ref="A130:A133"/>
-    <mergeCell ref="A134:A137"/>
-    <mergeCell ref="A138:A141"/>
-    <mergeCell ref="D124:D141"/>
-    <mergeCell ref="A125:A129"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>